<commit_message>
optical pimping of user list
</commit_message>
<xml_diff>
--- a/doc/User.xlsx
+++ b/doc/User.xlsx
@@ -7,19 +7,19 @@
     <workbookView xWindow="120" yWindow="120" windowWidth="24240" windowHeight="12075"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Liste SCM" sheetId="1" r:id="rId1"/>
+    <sheet name="Eingerichtete User" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$95</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Liste SCM'!$A$1:$K$95</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="270">
   <si>
     <t>AABDIN</t>
   </si>
@@ -468,13 +468,379 @@
   </si>
   <si>
     <t>ERODRIGU</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Stations</t>
+  </si>
+  <si>
+    <t>Is Staff</t>
+  </si>
+  <si>
+    <t>lmoppert</t>
+  </si>
+  <si>
+    <t>Lutz</t>
+  </si>
+  <si>
+    <t>Moppert</t>
+  </si>
+  <si>
+    <t>lutz.moppert@kronosww.com</t>
+  </si>
+  <si>
+    <t>Deutsch</t>
+  </si>
+  <si>
+    <t>administrator</t>
+  </si>
+  <si>
+    <t>Titanstraße</t>
+  </si>
+  <si>
+    <t>Werk Leverkusen</t>
+  </si>
+  <si>
+    <t>KRONOS Nordenham</t>
+  </si>
+  <si>
+    <t>Ghent</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>tellmann</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Ellmann</t>
+  </si>
+  <si>
+    <t>thomas.ellmann@kronosww.com</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>loadmaster</t>
+  </si>
+  <si>
+    <t>bmattheis</t>
+  </si>
+  <si>
+    <t>Birgit</t>
+  </si>
+  <si>
+    <t>Mattheis</t>
+  </si>
+  <si>
+    <t>birgit.mattheis@kronosww.com</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>hwohlfel</t>
+  </si>
+  <si>
+    <t>Harald</t>
+  </si>
+  <si>
+    <t>Wohlfeld</t>
+  </si>
+  <si>
+    <t>harald.wohlfeld@kronosww.com</t>
+  </si>
+  <si>
+    <t>cschmidt</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Schmidt</t>
+  </si>
+  <si>
+    <t>christian.schmidt@kronosww.com</t>
+  </si>
+  <si>
+    <t>erodrigu</t>
+  </si>
+  <si>
+    <t>Elsa</t>
+  </si>
+  <si>
+    <t>Rodrigues-Kloss</t>
+  </si>
+  <si>
+    <t>elsa.rodrigues-kloss@kronosww.com</t>
+  </si>
+  <si>
+    <t>rlongeri</t>
+  </si>
+  <si>
+    <t>Rita</t>
+  </si>
+  <si>
+    <t>Longerich</t>
+  </si>
+  <si>
+    <t>rita.longerich@kronosww.com</t>
+  </si>
+  <si>
+    <t>rschaefe</t>
+  </si>
+  <si>
+    <t>Ralf</t>
+  </si>
+  <si>
+    <t>Schäfer</t>
+  </si>
+  <si>
+    <t>ralf.schaefer@kronosww.com</t>
+  </si>
+  <si>
+    <t>charger</t>
+  </si>
+  <si>
+    <t>awild</t>
+  </si>
+  <si>
+    <t>Andreas</t>
+  </si>
+  <si>
+    <t>Wild</t>
+  </si>
+  <si>
+    <t>aabdin</t>
+  </si>
+  <si>
+    <t>Achim</t>
+  </si>
+  <si>
+    <t>Abdin</t>
+  </si>
+  <si>
+    <t>lmarkwart</t>
+  </si>
+  <si>
+    <t>Markwart</t>
+  </si>
+  <si>
+    <t>lutz.markwart@kronosww.com</t>
+  </si>
+  <si>
+    <t>jpenshor</t>
+  </si>
+  <si>
+    <t>Juergen</t>
+  </si>
+  <si>
+    <t>Penshorn</t>
+  </si>
+  <si>
+    <t>juergen.penshorn@kronosww.com</t>
+  </si>
+  <si>
+    <t>agerres</t>
+  </si>
+  <si>
+    <t>Annelies</t>
+  </si>
+  <si>
+    <t>Gerres</t>
+  </si>
+  <si>
+    <t>albers</t>
+  </si>
+  <si>
+    <t>avandenberghe</t>
+  </si>
+  <si>
+    <t>Anne</t>
+  </si>
+  <si>
+    <t>Vandenberghe</t>
+  </si>
+  <si>
+    <t>bertschi</t>
+  </si>
+  <si>
+    <t>mbilawa</t>
+  </si>
+  <si>
+    <t>viewer</t>
+  </si>
+  <si>
+    <t>blok</t>
+  </si>
+  <si>
+    <t>boezdede</t>
+  </si>
+  <si>
+    <t>Bahattin</t>
+  </si>
+  <si>
+    <t>Oezdede</t>
+  </si>
+  <si>
+    <t>chemion</t>
+  </si>
+  <si>
+    <t>dhl</t>
+  </si>
+  <si>
+    <t>dasbach</t>
+  </si>
+  <si>
+    <t>dasbach_du</t>
+  </si>
+  <si>
+    <t>buetefuehr_tank</t>
+  </si>
+  <si>
+    <t>ep_euro</t>
+  </si>
+  <si>
+    <t>lehnkering_euro</t>
+  </si>
+  <si>
+    <t>gdereu</t>
+  </si>
+  <si>
+    <t>greiwing</t>
+  </si>
+  <si>
+    <t>lalemant</t>
+  </si>
+  <si>
+    <t>lehnkering_tank</t>
+  </si>
+  <si>
+    <t>nolden</t>
+  </si>
+  <si>
+    <t>nsahan</t>
+  </si>
+  <si>
+    <t>Nurettin</t>
+  </si>
+  <si>
+    <t>Sahan</t>
+  </si>
+  <si>
+    <t>nurettin.sahan@kronosww.com</t>
+  </si>
+  <si>
+    <t>pdaub</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Daub</t>
+  </si>
+  <si>
+    <t>patrick.daub@kronosww.com</t>
+  </si>
+  <si>
+    <t>schmidt</t>
+  </si>
+  <si>
+    <t>bsiska</t>
+  </si>
+  <si>
+    <t>Bernd</t>
+  </si>
+  <si>
+    <t>Siska</t>
+  </si>
+  <si>
+    <t>bernd.siska@kronosww.com</t>
+  </si>
+  <si>
+    <t>ohl</t>
+  </si>
+  <si>
+    <t>reltrans_w</t>
+  </si>
+  <si>
+    <t>richter_tank</t>
+  </si>
+  <si>
+    <t>samskip</t>
+  </si>
+  <si>
+    <t>samskip_nl</t>
+  </si>
+  <si>
+    <t>schenker_a</t>
+  </si>
+  <si>
+    <t>schmidt_hn</t>
+  </si>
+  <si>
+    <t>talke_tank</t>
+  </si>
+  <si>
+    <t>transtrading</t>
+  </si>
+  <si>
+    <t>unifeeder</t>
+  </si>
+  <si>
+    <t>sun_global</t>
+  </si>
+  <si>
+    <t>lidercister</t>
+  </si>
+  <si>
+    <t>gus</t>
+  </si>
+  <si>
+    <t>konsor</t>
+  </si>
+  <si>
+    <t>van_der_lee</t>
+  </si>
+  <si>
+    <t>albers_logistik</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,8 +885,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -547,8 +926,20 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9F9F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -571,15 +962,115 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -597,10 +1088,62 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Berechnung" xfId="4" builtinId="22"/>
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -898,11 +1441,12 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T95"/>
+  <dimension ref="A1:R95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A95" sqref="A95:XFD95"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="P16" sqref="P16"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3267,15 +3811,2780 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A1" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="23">
+        <v>1</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="J3" s="24"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="J4" s="24"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="J5" s="24"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6" s="25"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="26">
+        <v>2</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="J8" s="27"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J9" s="27"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="J10" s="27"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="J11" s="28"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="23">
+        <v>7</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="J13" s="24"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="J14" s="24"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="J15" s="24"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" s="25"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="23">
+        <v>9</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="J18" s="24"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="J19" s="24"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="J20" s="24"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A21" s="25"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="J21" s="25"/>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A22" s="21">
+        <v>12</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="I22" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="J22" s="22" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="23">
+        <v>13</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="J23" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="J24" s="24"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="J25" s="24"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="J26" s="25"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A27" s="15">
+        <v>14</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="J27" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A28" s="13">
+        <v>15</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="J28" s="19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A29" s="15">
+        <v>16</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="I29" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="J29" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="23">
+        <v>17</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="H30" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="J30" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A31" s="25"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="J31" s="25"/>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A32" s="15">
+        <v>18</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="I32" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="J32" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="29.25" thickBot="1">
+      <c r="A33" s="13">
+        <v>19</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="J33" s="19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A34" s="15">
+        <v>20</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="H34" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="I34" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="J34" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A35" s="13">
+        <v>21</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="J35" s="19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="29.25" thickBot="1">
+      <c r="A36" s="21">
+        <v>22</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="H36" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="I36" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="J36" s="22" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="23">
+        <v>23</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="H37" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="J37" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A38" s="25"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="J38" s="25"/>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A39" s="15">
+        <v>24</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H39" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="J39" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="23">
+        <v>25</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H40" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="I40" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="J40" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="24"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="J41" s="24"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="24"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="J42" s="24"/>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A43" s="25"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="J43" s="25"/>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A44" s="15">
+        <v>26</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="I44" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="J44" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A45" s="13">
+        <v>28</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="I45" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="J45" s="19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="26">
+        <v>29</v>
+      </c>
+      <c r="B46" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="C46" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="H46" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="I46" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="J46" s="26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="27"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J47" s="27"/>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A48" s="28"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="28"/>
+      <c r="H48" s="28"/>
+      <c r="I48" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="J48" s="28"/>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="23">
+        <v>30</v>
+      </c>
+      <c r="B49" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="C49" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="H49" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="I49" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="J49" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A50" s="25"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="25"/>
+      <c r="I50" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="J50" s="25"/>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="26">
+        <v>31</v>
+      </c>
+      <c r="B51" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="H51" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="I51" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="J51" s="26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A52" s="28"/>
+      <c r="B52" s="28"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="J52" s="28"/>
+    </row>
+    <row r="53" spans="1:10" ht="29.25" thickBot="1">
+      <c r="A53" s="13">
+        <v>32</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="H53" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I53" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="J53" s="19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="26">
+        <v>33</v>
+      </c>
+      <c r="B54" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="C54" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="H54" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="I54" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="J54" s="26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="27"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="27"/>
+      <c r="I55" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J55" s="27"/>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="27"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="27"/>
+      <c r="F56" s="27"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="27"/>
+      <c r="I56" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="J56" s="27"/>
+    </row>
+    <row r="57" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A57" s="28"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="28"/>
+      <c r="G57" s="28"/>
+      <c r="H57" s="28"/>
+      <c r="I57" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="J57" s="28"/>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="23">
+        <v>34</v>
+      </c>
+      <c r="B58" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="C58" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="H58" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="I58" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="J58" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="24"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="24"/>
+      <c r="H59" s="24"/>
+      <c r="I59" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="J59" s="24"/>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="24"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="24"/>
+      <c r="H60" s="24"/>
+      <c r="I60" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="J60" s="24"/>
+    </row>
+    <row r="61" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A61" s="25"/>
+      <c r="B61" s="25"/>
+      <c r="C61" s="25"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="25"/>
+      <c r="F61" s="25"/>
+      <c r="G61" s="25"/>
+      <c r="H61" s="25"/>
+      <c r="I61" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="J61" s="25"/>
+    </row>
+    <row r="62" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A62" s="15">
+        <v>35</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="H62" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="I62" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="J62" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A63" s="13">
+        <v>36</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="H63" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I63" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="J63" s="19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A64" s="15">
+        <v>37</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="H64" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I64" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="J64" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="29.25" thickBot="1">
+      <c r="A65" s="13">
+        <v>38</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="H65" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I65" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="J65" s="19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="26">
+        <v>39</v>
+      </c>
+      <c r="B66" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="C66" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="D66" s="26"/>
+      <c r="E66" s="26"/>
+      <c r="F66" s="26"/>
+      <c r="G66" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="H66" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="I66" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="J66" s="26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="27"/>
+      <c r="B67" s="27"/>
+      <c r="C67" s="27"/>
+      <c r="D67" s="27"/>
+      <c r="E67" s="27"/>
+      <c r="F67" s="27"/>
+      <c r="G67" s="27"/>
+      <c r="H67" s="27"/>
+      <c r="I67" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J67" s="27"/>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="27"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="27"/>
+      <c r="E68" s="27"/>
+      <c r="F68" s="27"/>
+      <c r="G68" s="27"/>
+      <c r="H68" s="27"/>
+      <c r="I68" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="J68" s="27"/>
+    </row>
+    <row r="69" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A69" s="28"/>
+      <c r="B69" s="28"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="28"/>
+      <c r="E69" s="28"/>
+      <c r="F69" s="28"/>
+      <c r="G69" s="28"/>
+      <c r="H69" s="28"/>
+      <c r="I69" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="J69" s="28"/>
+    </row>
+    <row r="70" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A70" s="13">
+        <v>40</v>
+      </c>
+      <c r="B70" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D70" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="E70" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="F70" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="G70" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="H70" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="I70" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="J70" s="19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="26">
+        <v>41</v>
+      </c>
+      <c r="B71" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="C71" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D71" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="E71" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="F71" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="G71" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="H71" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="I71" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="J71" s="26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="27"/>
+      <c r="B72" s="27"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="27"/>
+      <c r="E72" s="27"/>
+      <c r="F72" s="27"/>
+      <c r="G72" s="27"/>
+      <c r="H72" s="27"/>
+      <c r="I72" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="J72" s="27"/>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="27"/>
+      <c r="B73" s="27"/>
+      <c r="C73" s="27"/>
+      <c r="D73" s="27"/>
+      <c r="E73" s="27"/>
+      <c r="F73" s="27"/>
+      <c r="G73" s="27"/>
+      <c r="H73" s="27"/>
+      <c r="I73" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J73" s="27"/>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="27"/>
+      <c r="B74" s="27"/>
+      <c r="C74" s="27"/>
+      <c r="D74" s="27"/>
+      <c r="E74" s="27"/>
+      <c r="F74" s="27"/>
+      <c r="G74" s="27"/>
+      <c r="H74" s="27"/>
+      <c r="I74" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="J74" s="27"/>
+    </row>
+    <row r="75" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A75" s="28"/>
+      <c r="B75" s="28"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="28"/>
+      <c r="F75" s="28"/>
+      <c r="G75" s="28"/>
+      <c r="H75" s="28"/>
+      <c r="I75" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="J75" s="28"/>
+    </row>
+    <row r="76" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A76" s="13">
+        <v>42</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="H76" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="I76" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="J76" s="19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A77" s="21">
+        <v>43</v>
+      </c>
+      <c r="B77" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="C77" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D77" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="E77" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="F77" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="G77" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="H77" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="I77" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="J77" s="22" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="23">
+        <v>44</v>
+      </c>
+      <c r="B78" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="C78" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="D78" s="23"/>
+      <c r="E78" s="23"/>
+      <c r="F78" s="23"/>
+      <c r="G78" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H78" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="I78" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="J78" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="24"/>
+      <c r="B79" s="24"/>
+      <c r="C79" s="24"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="24"/>
+      <c r="H79" s="24"/>
+      <c r="I79" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="J79" s="24"/>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="24"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="24"/>
+      <c r="D80" s="24"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="24"/>
+      <c r="G80" s="24"/>
+      <c r="H80" s="24"/>
+      <c r="I80" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="J80" s="24"/>
+    </row>
+    <row r="81" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A81" s="25"/>
+      <c r="B81" s="25"/>
+      <c r="C81" s="25"/>
+      <c r="D81" s="25"/>
+      <c r="E81" s="25"/>
+      <c r="F81" s="25"/>
+      <c r="G81" s="25"/>
+      <c r="H81" s="25"/>
+      <c r="I81" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="J81" s="25"/>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="26">
+        <v>45</v>
+      </c>
+      <c r="B82" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="C82" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="D82" s="26"/>
+      <c r="E82" s="26"/>
+      <c r="F82" s="26"/>
+      <c r="G82" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="H82" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="I82" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="J82" s="26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" s="27"/>
+      <c r="B83" s="27"/>
+      <c r="C83" s="27"/>
+      <c r="D83" s="27"/>
+      <c r="E83" s="27"/>
+      <c r="F83" s="27"/>
+      <c r="G83" s="27"/>
+      <c r="H83" s="27"/>
+      <c r="I83" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J83" s="27"/>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84" s="27"/>
+      <c r="B84" s="27"/>
+      <c r="C84" s="27"/>
+      <c r="D84" s="27"/>
+      <c r="E84" s="27"/>
+      <c r="F84" s="27"/>
+      <c r="G84" s="27"/>
+      <c r="H84" s="27"/>
+      <c r="I84" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="J84" s="27"/>
+    </row>
+    <row r="85" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A85" s="28"/>
+      <c r="B85" s="28"/>
+      <c r="C85" s="28"/>
+      <c r="D85" s="28"/>
+      <c r="E85" s="28"/>
+      <c r="F85" s="28"/>
+      <c r="G85" s="28"/>
+      <c r="H85" s="28"/>
+      <c r="I85" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="J85" s="28"/>
+    </row>
+    <row r="86" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A86" s="13">
+        <v>46</v>
+      </c>
+      <c r="B86" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="C86" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D86" s="13"/>
+      <c r="E86" s="13"/>
+      <c r="F86" s="13"/>
+      <c r="G86" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="H86" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I86" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="J86" s="19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" s="26">
+        <v>47</v>
+      </c>
+      <c r="B87" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="C87" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="D87" s="26"/>
+      <c r="E87" s="26"/>
+      <c r="F87" s="26"/>
+      <c r="G87" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="H87" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="I87" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="J87" s="26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88" s="27"/>
+      <c r="B88" s="27"/>
+      <c r="C88" s="27"/>
+      <c r="D88" s="27"/>
+      <c r="E88" s="27"/>
+      <c r="F88" s="27"/>
+      <c r="G88" s="27"/>
+      <c r="H88" s="27"/>
+      <c r="I88" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J88" s="27"/>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89" s="27"/>
+      <c r="B89" s="27"/>
+      <c r="C89" s="27"/>
+      <c r="D89" s="27"/>
+      <c r="E89" s="27"/>
+      <c r="F89" s="27"/>
+      <c r="G89" s="27"/>
+      <c r="H89" s="27"/>
+      <c r="I89" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="J89" s="27"/>
+    </row>
+    <row r="90" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A90" s="28"/>
+      <c r="B90" s="28"/>
+      <c r="C90" s="28"/>
+      <c r="D90" s="28"/>
+      <c r="E90" s="28"/>
+      <c r="F90" s="28"/>
+      <c r="G90" s="28"/>
+      <c r="H90" s="28"/>
+      <c r="I90" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="J90" s="28"/>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="23">
+        <v>48</v>
+      </c>
+      <c r="B91" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="C91" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="D91" s="23"/>
+      <c r="E91" s="23"/>
+      <c r="F91" s="23"/>
+      <c r="G91" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H91" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="I91" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="J91" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" s="24"/>
+      <c r="B92" s="24"/>
+      <c r="C92" s="24"/>
+      <c r="D92" s="24"/>
+      <c r="E92" s="24"/>
+      <c r="F92" s="24"/>
+      <c r="G92" s="24"/>
+      <c r="H92" s="24"/>
+      <c r="I92" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="J92" s="24"/>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" s="24"/>
+      <c r="B93" s="24"/>
+      <c r="C93" s="24"/>
+      <c r="D93" s="24"/>
+      <c r="E93" s="24"/>
+      <c r="F93" s="24"/>
+      <c r="G93" s="24"/>
+      <c r="H93" s="24"/>
+      <c r="I93" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="J93" s="24"/>
+    </row>
+    <row r="94" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A94" s="25"/>
+      <c r="B94" s="25"/>
+      <c r="C94" s="25"/>
+      <c r="D94" s="25"/>
+      <c r="E94" s="25"/>
+      <c r="F94" s="25"/>
+      <c r="G94" s="25"/>
+      <c r="H94" s="25"/>
+      <c r="I94" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="J94" s="25"/>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" s="26">
+        <v>49</v>
+      </c>
+      <c r="B95" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="C95" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D95" s="26"/>
+      <c r="E95" s="26"/>
+      <c r="F95" s="26"/>
+      <c r="G95" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="H95" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="I95" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="J95" s="26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96" s="27"/>
+      <c r="B96" s="27"/>
+      <c r="C96" s="27"/>
+      <c r="D96" s="27"/>
+      <c r="E96" s="27"/>
+      <c r="F96" s="27"/>
+      <c r="G96" s="27"/>
+      <c r="H96" s="27"/>
+      <c r="I96" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J96" s="27"/>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97" s="27"/>
+      <c r="B97" s="27"/>
+      <c r="C97" s="27"/>
+      <c r="D97" s="27"/>
+      <c r="E97" s="27"/>
+      <c r="F97" s="27"/>
+      <c r="G97" s="27"/>
+      <c r="H97" s="27"/>
+      <c r="I97" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="J97" s="27"/>
+    </row>
+    <row r="98" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A98" s="28"/>
+      <c r="B98" s="28"/>
+      <c r="C98" s="28"/>
+      <c r="D98" s="28"/>
+      <c r="E98" s="28"/>
+      <c r="F98" s="28"/>
+      <c r="G98" s="28"/>
+      <c r="H98" s="28"/>
+      <c r="I98" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="J98" s="28"/>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" s="23">
+        <v>50</v>
+      </c>
+      <c r="B99" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="C99" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D99" s="23"/>
+      <c r="E99" s="23"/>
+      <c r="F99" s="23"/>
+      <c r="G99" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="H99" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="I99" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="J99" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" s="24"/>
+      <c r="B100" s="24"/>
+      <c r="C100" s="24"/>
+      <c r="D100" s="24"/>
+      <c r="E100" s="24"/>
+      <c r="F100" s="24"/>
+      <c r="G100" s="24"/>
+      <c r="H100" s="24"/>
+      <c r="I100" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="J100" s="24"/>
+    </row>
+    <row r="101" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A101" s="25"/>
+      <c r="B101" s="25"/>
+      <c r="C101" s="25"/>
+      <c r="D101" s="25"/>
+      <c r="E101" s="25"/>
+      <c r="F101" s="25"/>
+      <c r="G101" s="25"/>
+      <c r="H101" s="25"/>
+      <c r="I101" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="J101" s="25"/>
+    </row>
+    <row r="102" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A102" s="15">
+        <v>51</v>
+      </c>
+      <c r="B102" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="C102" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D102" s="15"/>
+      <c r="E102" s="15"/>
+      <c r="F102" s="15"/>
+      <c r="G102" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H102" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I102" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="J102" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103" s="23">
+        <v>52</v>
+      </c>
+      <c r="B103" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="C103" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="D103" s="23"/>
+      <c r="E103" s="23"/>
+      <c r="F103" s="23"/>
+      <c r="G103" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="H103" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="I103" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="J103" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104" s="24"/>
+      <c r="B104" s="24"/>
+      <c r="C104" s="24"/>
+      <c r="D104" s="24"/>
+      <c r="E104" s="24"/>
+      <c r="F104" s="24"/>
+      <c r="G104" s="24"/>
+      <c r="H104" s="24"/>
+      <c r="I104" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="J104" s="24"/>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="A105" s="24"/>
+      <c r="B105" s="24"/>
+      <c r="C105" s="24"/>
+      <c r="D105" s="24"/>
+      <c r="E105" s="24"/>
+      <c r="F105" s="24"/>
+      <c r="G105" s="24"/>
+      <c r="H105" s="24"/>
+      <c r="I105" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="J105" s="24"/>
+    </row>
+    <row r="106" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A106" s="25"/>
+      <c r="B106" s="25"/>
+      <c r="C106" s="25"/>
+      <c r="D106" s="25"/>
+      <c r="E106" s="25"/>
+      <c r="F106" s="25"/>
+      <c r="G106" s="25"/>
+      <c r="H106" s="25"/>
+      <c r="I106" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="J106" s="25"/>
+    </row>
+    <row r="107" spans="1:10">
+      <c r="A107" s="26">
+        <v>53</v>
+      </c>
+      <c r="B107" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="C107" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="D107" s="26"/>
+      <c r="E107" s="26"/>
+      <c r="F107" s="26"/>
+      <c r="G107" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="H107" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="I107" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="J107" s="26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10">
+      <c r="A108" s="27"/>
+      <c r="B108" s="27"/>
+      <c r="C108" s="27"/>
+      <c r="D108" s="27"/>
+      <c r="E108" s="27"/>
+      <c r="F108" s="27"/>
+      <c r="G108" s="27"/>
+      <c r="H108" s="27"/>
+      <c r="I108" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J108" s="27"/>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109" s="27"/>
+      <c r="B109" s="27"/>
+      <c r="C109" s="27"/>
+      <c r="D109" s="27"/>
+      <c r="E109" s="27"/>
+      <c r="F109" s="27"/>
+      <c r="G109" s="27"/>
+      <c r="H109" s="27"/>
+      <c r="I109" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="J109" s="27"/>
+    </row>
+    <row r="110" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A110" s="28"/>
+      <c r="B110" s="28"/>
+      <c r="C110" s="28"/>
+      <c r="D110" s="28"/>
+      <c r="E110" s="28"/>
+      <c r="F110" s="28"/>
+      <c r="G110" s="28"/>
+      <c r="H110" s="28"/>
+      <c r="I110" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="J110" s="28"/>
+    </row>
+    <row r="111" spans="1:10">
+      <c r="A111" s="23">
+        <v>54</v>
+      </c>
+      <c r="B111" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="C111" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="D111" s="23"/>
+      <c r="E111" s="23"/>
+      <c r="F111" s="23"/>
+      <c r="G111" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="H111" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="I111" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="J111" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10">
+      <c r="A112" s="24"/>
+      <c r="B112" s="24"/>
+      <c r="C112" s="24"/>
+      <c r="D112" s="24"/>
+      <c r="E112" s="24"/>
+      <c r="F112" s="24"/>
+      <c r="G112" s="24"/>
+      <c r="H112" s="24"/>
+      <c r="I112" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="J112" s="24"/>
+    </row>
+    <row r="113" spans="1:10">
+      <c r="A113" s="24"/>
+      <c r="B113" s="24"/>
+      <c r="C113" s="24"/>
+      <c r="D113" s="24"/>
+      <c r="E113" s="24"/>
+      <c r="F113" s="24"/>
+      <c r="G113" s="24"/>
+      <c r="H113" s="24"/>
+      <c r="I113" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="J113" s="24"/>
+    </row>
+    <row r="114" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A114" s="25"/>
+      <c r="B114" s="25"/>
+      <c r="C114" s="25"/>
+      <c r="D114" s="25"/>
+      <c r="E114" s="25"/>
+      <c r="F114" s="25"/>
+      <c r="G114" s="25"/>
+      <c r="H114" s="25"/>
+      <c r="I114" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="J114" s="25"/>
+    </row>
+    <row r="115" spans="1:10">
+      <c r="A115" s="26">
+        <v>55</v>
+      </c>
+      <c r="B115" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="C115" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="D115" s="26"/>
+      <c r="E115" s="26"/>
+      <c r="F115" s="26"/>
+      <c r="G115" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="H115" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="I115" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="J115" s="26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10">
+      <c r="A116" s="27"/>
+      <c r="B116" s="27"/>
+      <c r="C116" s="27"/>
+      <c r="D116" s="27"/>
+      <c r="E116" s="27"/>
+      <c r="F116" s="27"/>
+      <c r="G116" s="27"/>
+      <c r="H116" s="27"/>
+      <c r="I116" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J116" s="27"/>
+    </row>
+    <row r="117" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A117" s="28"/>
+      <c r="B117" s="28"/>
+      <c r="C117" s="28"/>
+      <c r="D117" s="28"/>
+      <c r="E117" s="28"/>
+      <c r="F117" s="28"/>
+      <c r="G117" s="28"/>
+      <c r="H117" s="28"/>
+      <c r="I117" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="J117" s="28"/>
+    </row>
+    <row r="118" spans="1:10">
+      <c r="A118" s="23">
+        <v>56</v>
+      </c>
+      <c r="B118" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="C118" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D118" s="23"/>
+      <c r="E118" s="23"/>
+      <c r="F118" s="23"/>
+      <c r="G118" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="H118" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="I118" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="J118" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
+      <c r="A119" s="24"/>
+      <c r="B119" s="24"/>
+      <c r="C119" s="24"/>
+      <c r="D119" s="24"/>
+      <c r="E119" s="24"/>
+      <c r="F119" s="24"/>
+      <c r="G119" s="24"/>
+      <c r="H119" s="24"/>
+      <c r="I119" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="J119" s="24"/>
+    </row>
+    <row r="120" spans="1:10">
+      <c r="A120" s="24"/>
+      <c r="B120" s="24"/>
+      <c r="C120" s="24"/>
+      <c r="D120" s="24"/>
+      <c r="E120" s="24"/>
+      <c r="F120" s="24"/>
+      <c r="G120" s="24"/>
+      <c r="H120" s="24"/>
+      <c r="I120" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="J120" s="24"/>
+    </row>
+    <row r="121" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A121" s="25"/>
+      <c r="B121" s="25"/>
+      <c r="C121" s="25"/>
+      <c r="D121" s="25"/>
+      <c r="E121" s="25"/>
+      <c r="F121" s="25"/>
+      <c r="G121" s="25"/>
+      <c r="H121" s="25"/>
+      <c r="I121" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="J121" s="25"/>
+    </row>
+    <row r="122" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A122" s="15">
+        <v>57</v>
+      </c>
+      <c r="B122" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="C122" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D122" s="15"/>
+      <c r="E122" s="15"/>
+      <c r="F122" s="15"/>
+      <c r="G122" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H122" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I122" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="J122" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" ht="29.25" thickBot="1">
+      <c r="A123" s="13">
+        <v>58</v>
+      </c>
+      <c r="B123" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="C123" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D123" s="13"/>
+      <c r="E123" s="13"/>
+      <c r="F123" s="13"/>
+      <c r="G123" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="H123" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="I123" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="J123" s="19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10">
+      <c r="A124" s="26">
+        <v>59</v>
+      </c>
+      <c r="B124" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="C124" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="D124" s="26"/>
+      <c r="E124" s="26"/>
+      <c r="F124" s="26"/>
+      <c r="G124" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="H124" s="26"/>
+      <c r="I124" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="J124" s="26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10">
+      <c r="A125" s="27"/>
+      <c r="B125" s="27"/>
+      <c r="C125" s="27"/>
+      <c r="D125" s="27"/>
+      <c r="E125" s="27"/>
+      <c r="F125" s="27"/>
+      <c r="G125" s="27"/>
+      <c r="H125" s="27"/>
+      <c r="I125" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J125" s="27"/>
+    </row>
+    <row r="126" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A126" s="28"/>
+      <c r="B126" s="28"/>
+      <c r="C126" s="28"/>
+      <c r="D126" s="28"/>
+      <c r="E126" s="28"/>
+      <c r="F126" s="28"/>
+      <c r="G126" s="28"/>
+      <c r="H126" s="28"/>
+      <c r="I126" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="J126" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="243">
+    <mergeCell ref="J118:J121"/>
+    <mergeCell ref="A124:A126"/>
+    <mergeCell ref="B124:B126"/>
+    <mergeCell ref="C124:C126"/>
+    <mergeCell ref="D124:D126"/>
+    <mergeCell ref="E124:E126"/>
+    <mergeCell ref="F124:F126"/>
+    <mergeCell ref="G124:G126"/>
+    <mergeCell ref="H124:H126"/>
+    <mergeCell ref="J124:J126"/>
+    <mergeCell ref="H115:H117"/>
+    <mergeCell ref="J115:J117"/>
+    <mergeCell ref="A118:A121"/>
+    <mergeCell ref="B118:B121"/>
+    <mergeCell ref="C118:C121"/>
+    <mergeCell ref="D118:D121"/>
+    <mergeCell ref="E118:E121"/>
+    <mergeCell ref="F118:F121"/>
+    <mergeCell ref="G118:G121"/>
+    <mergeCell ref="H118:H121"/>
+    <mergeCell ref="G111:G114"/>
+    <mergeCell ref="H111:H114"/>
+    <mergeCell ref="J111:J114"/>
+    <mergeCell ref="A115:A117"/>
+    <mergeCell ref="B115:B117"/>
+    <mergeCell ref="C115:C117"/>
+    <mergeCell ref="D115:D117"/>
+    <mergeCell ref="E115:E117"/>
+    <mergeCell ref="F115:F117"/>
+    <mergeCell ref="G115:G117"/>
+    <mergeCell ref="A111:A114"/>
+    <mergeCell ref="B111:B114"/>
+    <mergeCell ref="C111:C114"/>
+    <mergeCell ref="D111:D114"/>
+    <mergeCell ref="E111:E114"/>
+    <mergeCell ref="F111:F114"/>
+    <mergeCell ref="J103:J106"/>
+    <mergeCell ref="A107:A110"/>
+    <mergeCell ref="B107:B110"/>
+    <mergeCell ref="C107:C110"/>
+    <mergeCell ref="D107:D110"/>
+    <mergeCell ref="E107:E110"/>
+    <mergeCell ref="F107:F110"/>
+    <mergeCell ref="G107:G110"/>
+    <mergeCell ref="H107:H110"/>
+    <mergeCell ref="J107:J110"/>
+    <mergeCell ref="H99:H101"/>
+    <mergeCell ref="J99:J101"/>
+    <mergeCell ref="A103:A106"/>
+    <mergeCell ref="B103:B106"/>
+    <mergeCell ref="C103:C106"/>
+    <mergeCell ref="D103:D106"/>
+    <mergeCell ref="E103:E106"/>
+    <mergeCell ref="F103:F106"/>
+    <mergeCell ref="G103:G106"/>
+    <mergeCell ref="H103:H106"/>
+    <mergeCell ref="G95:G98"/>
+    <mergeCell ref="H95:H98"/>
+    <mergeCell ref="J95:J98"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="C99:C101"/>
+    <mergeCell ref="D99:D101"/>
+    <mergeCell ref="E99:E101"/>
+    <mergeCell ref="F99:F101"/>
+    <mergeCell ref="G99:G101"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="B95:B98"/>
+    <mergeCell ref="C95:C98"/>
+    <mergeCell ref="D95:D98"/>
+    <mergeCell ref="E95:E98"/>
+    <mergeCell ref="F95:F98"/>
+    <mergeCell ref="J87:J90"/>
+    <mergeCell ref="A91:A94"/>
+    <mergeCell ref="B91:B94"/>
+    <mergeCell ref="C91:C94"/>
+    <mergeCell ref="D91:D94"/>
+    <mergeCell ref="E91:E94"/>
+    <mergeCell ref="F91:F94"/>
+    <mergeCell ref="G91:G94"/>
+    <mergeCell ref="H91:H94"/>
+    <mergeCell ref="J91:J94"/>
+    <mergeCell ref="H82:H85"/>
+    <mergeCell ref="J82:J85"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="B87:B90"/>
+    <mergeCell ref="C87:C90"/>
+    <mergeCell ref="D87:D90"/>
+    <mergeCell ref="E87:E90"/>
+    <mergeCell ref="F87:F90"/>
+    <mergeCell ref="G87:G90"/>
+    <mergeCell ref="H87:H90"/>
+    <mergeCell ref="G78:G81"/>
+    <mergeCell ref="H78:H81"/>
+    <mergeCell ref="J78:J81"/>
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="C82:C85"/>
+    <mergeCell ref="D82:D85"/>
+    <mergeCell ref="E82:E85"/>
+    <mergeCell ref="F82:F85"/>
+    <mergeCell ref="G82:G85"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="C78:C81"/>
+    <mergeCell ref="D78:D81"/>
+    <mergeCell ref="E78:E81"/>
+    <mergeCell ref="F78:F81"/>
+    <mergeCell ref="J66:J69"/>
+    <mergeCell ref="A71:A75"/>
+    <mergeCell ref="B71:B75"/>
+    <mergeCell ref="C71:C75"/>
+    <mergeCell ref="D71:D75"/>
+    <mergeCell ref="E71:E75"/>
+    <mergeCell ref="F71:F75"/>
+    <mergeCell ref="G71:G75"/>
+    <mergeCell ref="H71:H75"/>
+    <mergeCell ref="J71:J75"/>
+    <mergeCell ref="H58:H61"/>
+    <mergeCell ref="J58:J61"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="E66:E69"/>
+    <mergeCell ref="F66:F69"/>
+    <mergeCell ref="G66:G69"/>
+    <mergeCell ref="H66:H69"/>
+    <mergeCell ref="G54:G57"/>
+    <mergeCell ref="H54:H57"/>
+    <mergeCell ref="J54:J57"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="D58:D61"/>
+    <mergeCell ref="E58:E61"/>
+    <mergeCell ref="F58:F61"/>
+    <mergeCell ref="G58:G61"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="D54:D57"/>
+    <mergeCell ref="E54:E57"/>
+    <mergeCell ref="F54:F57"/>
+    <mergeCell ref="J49:J50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="J51:J52"/>
+    <mergeCell ref="H46:H48"/>
+    <mergeCell ref="J46:J48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="G40:G43"/>
+    <mergeCell ref="H40:H43"/>
+    <mergeCell ref="J40:J43"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="G46:G48"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="F40:F43"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="J37:J38"/>
+    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="J23:J26"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="J17:J21"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="D17:D21"/>
+    <mergeCell ref="E17:E21"/>
+    <mergeCell ref="F17:F21"/>
+    <mergeCell ref="G17:G21"/>
+    <mergeCell ref="H17:H21"/>
+    <mergeCell ref="G12:G16"/>
+    <mergeCell ref="H12:H16"/>
+    <mergeCell ref="J12:J16"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="E12:E16"/>
+    <mergeCell ref="F12:F16"/>
+    <mergeCell ref="H7:H11"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="G2:G6"/>
+    <mergeCell ref="H2:H6"/>
+    <mergeCell ref="J2:J6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="E2:E6"/>
+    <mergeCell ref="F2:F6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="http://timeslots.eu.nli.net/timeslots/users/?sort=id"/>
+    <hyperlink ref="B1" r:id="rId2" display="http://timeslots.eu.nli.net/timeslots/users/?sort=username"/>
+    <hyperlink ref="C1" r:id="rId3" display="http://timeslots.eu.nli.net/timeslots/users/?sort=company"/>
+    <hyperlink ref="D1" r:id="rId4" display="http://timeslots.eu.nli.net/timeslots/users/?sort=firstname"/>
+    <hyperlink ref="E1" r:id="rId5" display="http://timeslots.eu.nli.net/timeslots/users/?sort=lastname"/>
+    <hyperlink ref="F1" r:id="rId6" display="http://timeslots.eu.nli.net/timeslots/users/?sort=email"/>
+    <hyperlink ref="G1" r:id="rId7" display="http://timeslots.eu.nli.net/timeslots/users/?sort=language"/>
+    <hyperlink ref="H1" r:id="rId8" display="http://timeslots.eu.nli.net/timeslots/users/?sort=group"/>
+    <hyperlink ref="I1" r:id="rId9" display="http://timeslots.eu.nli.net/timeslots/users/?sort=stations"/>
+    <hyperlink ref="J1" r:id="rId10" display="http://timeslots.eu.nli.net/timeslots/users/?sort=is_staff"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -3283,7 +6592,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>

<commit_message>
updated docs and user list
</commit_message>
<xml_diff>
--- a/doc/User.xlsx
+++ b/doc/User.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Liste SCM" sheetId="1" r:id="rId1"/>
     <sheet name="Eingerichtete User" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Berechtigungen" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Liste SCM'!$A$1:$K$95</definedName>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="281">
   <si>
     <t>AABDIN</t>
   </si>
@@ -834,13 +834,46 @@
   </si>
   <si>
     <t>albers_logistik</t>
+  </si>
+  <si>
+    <t>Einem User gehört genau einer Gruppe an und er hat die entsprechenden Rechte auf allen (!) Stationen, die Ihm zugeordnet sind.</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>Ladefenster blocken</t>
+  </si>
+  <si>
+    <t>Ladefenster bearbeiten (Nach Fristende)</t>
+  </si>
+  <si>
+    <t>Ladefenster bearbeiten (Fristgerecht)</t>
+  </si>
+  <si>
+    <t>Ladestatus bearbeiten</t>
+  </si>
+  <si>
+    <t>Fremde Einträge sehen</t>
+  </si>
+  <si>
+    <t>Eigene Einträge sehen</t>
+  </si>
+  <si>
+    <t>Mögliche Gruppen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -898,8 +931,32 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -935,6 +992,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF9F9F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1070,7 +1133,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1118,6 +1181,9 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1136,8 +1202,17 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1444,9 +1519,9 @@
   <dimension ref="A1:R95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P16" sqref="P16"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="A93" sqref="A93:XFD93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1762,30 +1837,30 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="8" customFormat="1">
-      <c r="A10" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="8" t="s">
+    <row r="10" spans="1:18" s="3" customFormat="1">
+      <c r="A10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="8" t="s">
+      <c r="F10" s="7"/>
+      <c r="G10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="L10" s="8" t="s">
+      <c r="L10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="R10" s="8" t="s">
+      <c r="R10" s="3" t="s">
         <v>139</v>
       </c>
     </row>
@@ -3195,30 +3270,30 @@
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:18" s="8" customFormat="1">
-      <c r="A71" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B71" s="8" t="s">
+    <row r="71" spans="1:18" s="3" customFormat="1">
+      <c r="A71" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E71" s="8" t="s">
+      <c r="E71" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F71" s="9"/>
-      <c r="G71" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H71" s="9"/>
-      <c r="I71" s="9"/>
-      <c r="J71" s="9"/>
-      <c r="K71" s="8" t="s">
+      <c r="F71" s="7"/>
+      <c r="G71" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H71" s="7"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="L71" s="8" t="s">
+      <c r="L71" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="R71" s="8" t="s">
+      <c r="R71" s="3" t="s">
         <v>139</v>
       </c>
     </row>
@@ -3700,30 +3775,30 @@
         <v>139</v>
       </c>
     </row>
-    <row r="93" spans="1:18" s="8" customFormat="1">
-      <c r="A93" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B93" s="8" t="s">
+    <row r="93" spans="1:18" s="3" customFormat="1">
+      <c r="A93" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B93" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E93" s="8" t="s">
+      <c r="E93" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F93" s="9"/>
-      <c r="G93" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H93" s="9"/>
-      <c r="I93" s="9"/>
-      <c r="J93" s="9"/>
-      <c r="K93" s="8" t="s">
+      <c r="F93" s="7"/>
+      <c r="G93" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H93" s="7"/>
+      <c r="I93" s="7"/>
+      <c r="J93" s="7"/>
+      <c r="K93" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="L93" s="8" t="s">
+      <c r="L93" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="R93" s="8" t="s">
+      <c r="R93" s="3" t="s">
         <v>139</v>
       </c>
     </row>
@@ -3813,7 +3888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J126"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
@@ -3862,356 +3937,356 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="23">
+      <c r="A2" s="24">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="24" t="s">
         <v>163</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="24" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
       <c r="I3" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="J3" s="24"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="J4" s="24"/>
+      <c r="J4" s="25"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
       <c r="I5" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="J5" s="24"/>
+      <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
       <c r="I6" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J6" s="25"/>
+      <c r="J6" s="26"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="26">
+      <c r="A7" s="27">
         <v>2</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="27" t="s">
         <v>170</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="27" t="s">
         <v>163</v>
       </c>
       <c r="I7" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="27" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
       <c r="I8" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="J8" s="27"/>
+      <c r="J8" s="28"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
       <c r="I9" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="J9" s="27"/>
+      <c r="J9" s="28"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
       <c r="I10" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="J10" s="27"/>
+      <c r="J10" s="28"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
       <c r="I11" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="J11" s="28"/>
+      <c r="J11" s="29"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="23">
+      <c r="A12" s="24">
         <v>7</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="24" t="s">
         <v>163</v>
       </c>
       <c r="I12" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="J12" s="23" t="s">
+      <c r="J12" s="24" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
       <c r="I13" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="J13" s="24"/>
+      <c r="J13" s="25"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
       <c r="I14" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="J14" s="24"/>
+      <c r="J14" s="25"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
       <c r="I15" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="J15" s="24"/>
+      <c r="J15" s="25"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
       <c r="I16" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J16" s="25"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="23">
+      <c r="A17" s="24">
         <v>9</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="E17" s="23" t="s">
+      <c r="E17" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="G17" s="23" t="s">
+      <c r="G17" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="H17" s="23" t="s">
+      <c r="H17" s="24" t="s">
         <v>163</v>
       </c>
       <c r="I17" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="J17" s="23" t="s">
+      <c r="J17" s="24" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="24"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
       <c r="I18" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="J18" s="24"/>
+      <c r="J18" s="25"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
       <c r="I19" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="J19" s="24"/>
+      <c r="J19" s="25"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="24"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
       <c r="I20" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="J20" s="24"/>
+      <c r="J20" s="25"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A21" s="25"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
       <c r="I21" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J21" s="25"/>
+      <c r="J21" s="26"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1">
       <c r="A22" s="21">
@@ -4246,78 +4321,78 @@
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="23">
+      <c r="A23" s="24">
         <v>13</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="23" t="s">
+      <c r="D23" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="E23" s="23" t="s">
+      <c r="E23" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="F23" s="23" t="s">
+      <c r="F23" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="23" t="s">
+      <c r="G23" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="H23" s="23" t="s">
+      <c r="H23" s="24" t="s">
         <v>173</v>
       </c>
       <c r="I23" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="J23" s="23" t="s">
+      <c r="J23" s="24" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
       <c r="I24" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="J24" s="24"/>
+      <c r="J24" s="25"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
       <c r="I25" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="J25" s="24"/>
+      <c r="J25" s="25"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
       <c r="I26" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J26" s="25"/>
+      <c r="J26" s="26"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" thickBot="1">
       <c r="A27" s="15">
@@ -4416,50 +4491,50 @@
       </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="23">
+      <c r="A30" s="24">
         <v>17</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D30" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="F30" s="23" t="s">
+      <c r="F30" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="G30" s="23" t="s">
+      <c r="G30" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="H30" s="23" t="s">
+      <c r="H30" s="24" t="s">
         <v>175</v>
       </c>
       <c r="I30" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="J30" s="23" t="s">
+      <c r="J30" s="24" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A31" s="25"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
       <c r="I31" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J31" s="25"/>
+      <c r="J31" s="26"/>
     </row>
     <row r="32" spans="1:10" ht="15.75" thickBot="1">
       <c r="A32" s="15">
@@ -4493,7 +4568,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="29.25" thickBot="1">
+    <row r="33" spans="1:10" ht="15.75" thickBot="1">
       <c r="A33" s="13">
         <v>19</v>
       </c>
@@ -4614,44 +4689,44 @@
       </c>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="23">
+      <c r="A37" s="24">
         <v>23</v>
       </c>
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="24" t="s">
         <v>222</v>
       </c>
-      <c r="C37" s="23" t="s">
+      <c r="C37" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23" t="s">
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="H37" s="23" t="s">
+      <c r="H37" s="24" t="s">
         <v>173</v>
       </c>
       <c r="I37" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="J37" s="23" t="s">
+      <c r="J37" s="24" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A38" s="25"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
       <c r="I38" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="J38" s="25"/>
+      <c r="J38" s="26"/>
     </row>
     <row r="39" spans="1:10" ht="15.75" thickBot="1">
       <c r="A39" s="15">
@@ -4680,72 +4755,72 @@
       </c>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="23">
+      <c r="A40" s="24">
         <v>25</v>
       </c>
-      <c r="B40" s="23" t="s">
+      <c r="B40" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="C40" s="23" t="s">
+      <c r="C40" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="23" t="s">
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24" t="s">
         <v>180</v>
       </c>
-      <c r="H40" s="23" t="s">
+      <c r="H40" s="24" t="s">
         <v>173</v>
       </c>
       <c r="I40" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="J40" s="23" t="s">
+      <c r="J40" s="24" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="24"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="24"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="25"/>
       <c r="I41" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="J41" s="24"/>
+      <c r="J41" s="25"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="24"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
+      <c r="A42" s="25"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25"/>
       <c r="I42" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="J42" s="24"/>
+      <c r="J42" s="25"/>
     </row>
     <row r="43" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A43" s="25"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
       <c r="I43" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J43" s="25"/>
+      <c r="J43" s="26"/>
     </row>
     <row r="44" spans="1:10" ht="15.75" thickBot="1">
       <c r="A44" s="15">
@@ -4804,138 +4879,138 @@
       </c>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="26">
+      <c r="A46" s="27">
         <v>29</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="C46" s="26" t="s">
+      <c r="C46" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26" t="s">
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="H46" s="26" t="s">
+      <c r="H46" s="27" t="s">
         <v>173</v>
       </c>
       <c r="I46" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="J46" s="26" t="s">
+      <c r="J46" s="27" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="27"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
+      <c r="A47" s="28"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="28"/>
       <c r="I47" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="J47" s="27"/>
+      <c r="J47" s="28"/>
     </row>
     <row r="48" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A48" s="28"/>
-      <c r="B48" s="28"/>
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="28"/>
-      <c r="F48" s="28"/>
-      <c r="G48" s="28"/>
-      <c r="H48" s="28"/>
+      <c r="A48" s="29"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="29"/>
       <c r="I48" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="J48" s="28"/>
+      <c r="J48" s="29"/>
     </row>
     <row r="49" spans="1:10">
-      <c r="A49" s="23">
+      <c r="A49" s="24">
         <v>30</v>
       </c>
-      <c r="B49" s="23" t="s">
+      <c r="B49" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="C49" s="23" t="s">
+      <c r="C49" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="23" t="s">
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="H49" s="23" t="s">
+      <c r="H49" s="24" t="s">
         <v>173</v>
       </c>
       <c r="I49" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="J49" s="23" t="s">
+      <c r="J49" s="24" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A50" s="25"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="25"/>
-      <c r="H50" s="25"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
       <c r="I50" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="J50" s="25"/>
+      <c r="J50" s="26"/>
     </row>
     <row r="51" spans="1:10">
-      <c r="A51" s="26">
+      <c r="A51" s="27">
         <v>31</v>
       </c>
-      <c r="B51" s="26" t="s">
+      <c r="B51" s="27" t="s">
         <v>232</v>
       </c>
-      <c r="C51" s="26" t="s">
+      <c r="C51" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="26" t="s">
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="H51" s="26" t="s">
+      <c r="H51" s="27" t="s">
         <v>173</v>
       </c>
       <c r="I51" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="J51" s="26" t="s">
+      <c r="J51" s="27" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A52" s="28"/>
-      <c r="B52" s="28"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="28"/>
-      <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="28"/>
-      <c r="H52" s="28"/>
+      <c r="A52" s="29"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="29"/>
       <c r="I52" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="J52" s="28"/>
+      <c r="J52" s="29"/>
     </row>
     <row r="53" spans="1:10" ht="29.25" thickBot="1">
       <c r="A53" s="13">
@@ -4964,140 +5039,140 @@
       </c>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" s="26">
+      <c r="A54" s="27">
         <v>33</v>
       </c>
-      <c r="B54" s="26" t="s">
+      <c r="B54" s="27" t="s">
         <v>234</v>
       </c>
-      <c r="C54" s="26" t="s">
+      <c r="C54" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="26"/>
-      <c r="G54" s="26" t="s">
+      <c r="D54" s="27"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="H54" s="26" t="s">
+      <c r="H54" s="27" t="s">
         <v>173</v>
       </c>
       <c r="I54" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="J54" s="26" t="s">
+      <c r="J54" s="27" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="27"/>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="27"/>
-      <c r="H55" s="27"/>
+      <c r="A55" s="28"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28"/>
+      <c r="G55" s="28"/>
+      <c r="H55" s="28"/>
       <c r="I55" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="J55" s="27"/>
+      <c r="J55" s="28"/>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="27"/>
-      <c r="B56" s="27"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="27"/>
+      <c r="A56" s="28"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="28"/>
+      <c r="H56" s="28"/>
       <c r="I56" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="J56" s="27"/>
+      <c r="J56" s="28"/>
     </row>
     <row r="57" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A57" s="28"/>
-      <c r="B57" s="28"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="28"/>
-      <c r="G57" s="28"/>
-      <c r="H57" s="28"/>
-      <c r="I57" s="29" t="s">
+      <c r="A57" s="29"/>
+      <c r="B57" s="29"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="29"/>
+      <c r="G57" s="29"/>
+      <c r="H57" s="29"/>
+      <c r="I57" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="J57" s="28"/>
+      <c r="J57" s="29"/>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="23">
+      <c r="A58" s="24">
         <v>34</v>
       </c>
-      <c r="B58" s="23" t="s">
+      <c r="B58" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="C58" s="23" t="s">
+      <c r="C58" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="D58" s="23"/>
-      <c r="E58" s="23"/>
-      <c r="F58" s="23"/>
-      <c r="G58" s="23" t="s">
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="H58" s="23" t="s">
+      <c r="H58" s="24" t="s">
         <v>173</v>
       </c>
       <c r="I58" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="J58" s="23" t="s">
+      <c r="J58" s="24" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="24"/>
-      <c r="B59" s="24"/>
-      <c r="C59" s="24"/>
-      <c r="D59" s="24"/>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24"/>
-      <c r="G59" s="24"/>
-      <c r="H59" s="24"/>
+      <c r="A59" s="25"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="25"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="25"/>
+      <c r="F59" s="25"/>
+      <c r="G59" s="25"/>
+      <c r="H59" s="25"/>
       <c r="I59" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="J59" s="24"/>
+      <c r="J59" s="25"/>
     </row>
     <row r="60" spans="1:10">
-      <c r="A60" s="24"/>
-      <c r="B60" s="24"/>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
-      <c r="G60" s="24"/>
-      <c r="H60" s="24"/>
+      <c r="A60" s="25"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="25"/>
+      <c r="G60" s="25"/>
+      <c r="H60" s="25"/>
       <c r="I60" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="J60" s="24"/>
+      <c r="J60" s="25"/>
     </row>
     <row r="61" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A61" s="25"/>
-      <c r="B61" s="25"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="25"/>
-      <c r="G61" s="25"/>
-      <c r="H61" s="25"/>
+      <c r="A61" s="26"/>
+      <c r="B61" s="26"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
       <c r="I61" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J61" s="25"/>
+      <c r="J61" s="26"/>
     </row>
     <row r="62" spans="1:10" ht="15.75" thickBot="1">
       <c r="A62" s="15">
@@ -5177,7 +5252,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="29.25" thickBot="1">
+    <row r="65" spans="1:10" ht="15.75" thickBot="1">
       <c r="A65" s="13">
         <v>38</v>
       </c>
@@ -5204,72 +5279,72 @@
       </c>
     </row>
     <row r="66" spans="1:10">
-      <c r="A66" s="26">
+      <c r="A66" s="27">
         <v>39</v>
       </c>
-      <c r="B66" s="26" t="s">
+      <c r="B66" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="C66" s="26" t="s">
+      <c r="C66" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="D66" s="26"/>
-      <c r="E66" s="26"/>
-      <c r="F66" s="26"/>
-      <c r="G66" s="26" t="s">
+      <c r="D66" s="27"/>
+      <c r="E66" s="27"/>
+      <c r="F66" s="27"/>
+      <c r="G66" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="H66" s="26" t="s">
+      <c r="H66" s="27" t="s">
         <v>173</v>
       </c>
       <c r="I66" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="J66" s="26" t="s">
+      <c r="J66" s="27" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="67" spans="1:10">
-      <c r="A67" s="27"/>
-      <c r="B67" s="27"/>
-      <c r="C67" s="27"/>
-      <c r="D67" s="27"/>
-      <c r="E67" s="27"/>
-      <c r="F67" s="27"/>
-      <c r="G67" s="27"/>
-      <c r="H67" s="27"/>
+      <c r="A67" s="28"/>
+      <c r="B67" s="28"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="28"/>
+      <c r="G67" s="28"/>
+      <c r="H67" s="28"/>
       <c r="I67" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="J67" s="27"/>
+      <c r="J67" s="28"/>
     </row>
     <row r="68" spans="1:10">
-      <c r="A68" s="27"/>
-      <c r="B68" s="27"/>
-      <c r="C68" s="27"/>
-      <c r="D68" s="27"/>
-      <c r="E68" s="27"/>
-      <c r="F68" s="27"/>
-      <c r="G68" s="27"/>
-      <c r="H68" s="27"/>
+      <c r="A68" s="28"/>
+      <c r="B68" s="28"/>
+      <c r="C68" s="28"/>
+      <c r="D68" s="28"/>
+      <c r="E68" s="28"/>
+      <c r="F68" s="28"/>
+      <c r="G68" s="28"/>
+      <c r="H68" s="28"/>
       <c r="I68" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="J68" s="27"/>
+      <c r="J68" s="28"/>
     </row>
     <row r="69" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A69" s="28"/>
-      <c r="B69" s="28"/>
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
-      <c r="G69" s="28"/>
-      <c r="H69" s="28"/>
+      <c r="A69" s="29"/>
+      <c r="B69" s="29"/>
+      <c r="C69" s="29"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="29"/>
+      <c r="F69" s="29"/>
+      <c r="G69" s="29"/>
+      <c r="H69" s="29"/>
       <c r="I69" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="J69" s="28"/>
+      <c r="J69" s="29"/>
     </row>
     <row r="70" spans="1:10" ht="15.75" thickBot="1">
       <c r="A70" s="13">
@@ -5304,92 +5379,92 @@
       </c>
     </row>
     <row r="71" spans="1:10">
-      <c r="A71" s="26">
+      <c r="A71" s="27">
         <v>41</v>
       </c>
-      <c r="B71" s="26" t="s">
+      <c r="B71" s="27" t="s">
         <v>245</v>
       </c>
-      <c r="C71" s="26" t="s">
+      <c r="C71" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="D71" s="26" t="s">
+      <c r="D71" s="27" t="s">
         <v>246</v>
       </c>
-      <c r="E71" s="26" t="s">
+      <c r="E71" s="27" t="s">
         <v>247</v>
       </c>
-      <c r="F71" s="26" t="s">
+      <c r="F71" s="27" t="s">
         <v>248</v>
       </c>
-      <c r="G71" s="26" t="s">
+      <c r="G71" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="H71" s="26" t="s">
+      <c r="H71" s="27" t="s">
         <v>163</v>
       </c>
       <c r="I71" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="J71" s="26" t="s">
+      <c r="J71" s="27" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:10">
-      <c r="A72" s="27"/>
-      <c r="B72" s="27"/>
-      <c r="C72" s="27"/>
-      <c r="D72" s="27"/>
-      <c r="E72" s="27"/>
-      <c r="F72" s="27"/>
-      <c r="G72" s="27"/>
-      <c r="H72" s="27"/>
+      <c r="A72" s="28"/>
+      <c r="B72" s="28"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="28"/>
+      <c r="F72" s="28"/>
+      <c r="G72" s="28"/>
+      <c r="H72" s="28"/>
       <c r="I72" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="J72" s="27"/>
+      <c r="J72" s="28"/>
     </row>
     <row r="73" spans="1:10">
-      <c r="A73" s="27"/>
-      <c r="B73" s="27"/>
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
-      <c r="E73" s="27"/>
-      <c r="F73" s="27"/>
-      <c r="G73" s="27"/>
-      <c r="H73" s="27"/>
+      <c r="A73" s="28"/>
+      <c r="B73" s="28"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="28"/>
+      <c r="F73" s="28"/>
+      <c r="G73" s="28"/>
+      <c r="H73" s="28"/>
       <c r="I73" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="J73" s="27"/>
+      <c r="J73" s="28"/>
     </row>
     <row r="74" spans="1:10">
-      <c r="A74" s="27"/>
-      <c r="B74" s="27"/>
-      <c r="C74" s="27"/>
-      <c r="D74" s="27"/>
-      <c r="E74" s="27"/>
-      <c r="F74" s="27"/>
-      <c r="G74" s="27"/>
-      <c r="H74" s="27"/>
+      <c r="A74" s="28"/>
+      <c r="B74" s="28"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="28"/>
+      <c r="E74" s="28"/>
+      <c r="F74" s="28"/>
+      <c r="G74" s="28"/>
+      <c r="H74" s="28"/>
       <c r="I74" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="J74" s="27"/>
+      <c r="J74" s="28"/>
     </row>
     <row r="75" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A75" s="28"/>
-      <c r="B75" s="28"/>
-      <c r="C75" s="28"/>
-      <c r="D75" s="28"/>
-      <c r="E75" s="28"/>
-      <c r="F75" s="28"/>
-      <c r="G75" s="28"/>
-      <c r="H75" s="28"/>
+      <c r="A75" s="29"/>
+      <c r="B75" s="29"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="29"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="29"/>
+      <c r="G75" s="29"/>
+      <c r="H75" s="29"/>
       <c r="I75" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="J75" s="28"/>
+      <c r="J75" s="29"/>
     </row>
     <row r="76" spans="1:10" ht="15.75" thickBot="1">
       <c r="A76" s="13">
@@ -5450,140 +5525,140 @@
       </c>
     </row>
     <row r="78" spans="1:10">
-      <c r="A78" s="23">
+      <c r="A78" s="24">
         <v>44</v>
       </c>
-      <c r="B78" s="23" t="s">
+      <c r="B78" s="24" t="s">
         <v>254</v>
       </c>
-      <c r="C78" s="23" t="s">
+      <c r="C78" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D78" s="23"/>
-      <c r="E78" s="23"/>
-      <c r="F78" s="23"/>
-      <c r="G78" s="23" t="s">
+      <c r="D78" s="24"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="24"/>
+      <c r="G78" s="24" t="s">
         <v>180</v>
       </c>
-      <c r="H78" s="23" t="s">
+      <c r="H78" s="24" t="s">
         <v>173</v>
       </c>
       <c r="I78" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="J78" s="23" t="s">
+      <c r="J78" s="24" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="79" spans="1:10">
-      <c r="A79" s="24"/>
-      <c r="B79" s="24"/>
-      <c r="C79" s="24"/>
-      <c r="D79" s="24"/>
-      <c r="E79" s="24"/>
-      <c r="F79" s="24"/>
-      <c r="G79" s="24"/>
-      <c r="H79" s="24"/>
+      <c r="A79" s="25"/>
+      <c r="B79" s="25"/>
+      <c r="C79" s="25"/>
+      <c r="D79" s="25"/>
+      <c r="E79" s="25"/>
+      <c r="F79" s="25"/>
+      <c r="G79" s="25"/>
+      <c r="H79" s="25"/>
       <c r="I79" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="J79" s="24"/>
+      <c r="J79" s="25"/>
     </row>
     <row r="80" spans="1:10">
-      <c r="A80" s="24"/>
-      <c r="B80" s="24"/>
-      <c r="C80" s="24"/>
-      <c r="D80" s="24"/>
-      <c r="E80" s="24"/>
-      <c r="F80" s="24"/>
-      <c r="G80" s="24"/>
-      <c r="H80" s="24"/>
+      <c r="A80" s="25"/>
+      <c r="B80" s="25"/>
+      <c r="C80" s="25"/>
+      <c r="D80" s="25"/>
+      <c r="E80" s="25"/>
+      <c r="F80" s="25"/>
+      <c r="G80" s="25"/>
+      <c r="H80" s="25"/>
       <c r="I80" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="J80" s="24"/>
+      <c r="J80" s="25"/>
     </row>
     <row r="81" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A81" s="25"/>
-      <c r="B81" s="25"/>
-      <c r="C81" s="25"/>
-      <c r="D81" s="25"/>
-      <c r="E81" s="25"/>
-      <c r="F81" s="25"/>
-      <c r="G81" s="25"/>
-      <c r="H81" s="25"/>
+      <c r="A81" s="26"/>
+      <c r="B81" s="26"/>
+      <c r="C81" s="26"/>
+      <c r="D81" s="26"/>
+      <c r="E81" s="26"/>
+      <c r="F81" s="26"/>
+      <c r="G81" s="26"/>
+      <c r="H81" s="26"/>
       <c r="I81" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J81" s="25"/>
+      <c r="J81" s="26"/>
     </row>
     <row r="82" spans="1:10">
-      <c r="A82" s="26">
+      <c r="A82" s="27">
         <v>45</v>
       </c>
-      <c r="B82" s="26" t="s">
+      <c r="B82" s="27" t="s">
         <v>255</v>
       </c>
-      <c r="C82" s="26" t="s">
+      <c r="C82" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="D82" s="26"/>
-      <c r="E82" s="26"/>
-      <c r="F82" s="26"/>
-      <c r="G82" s="26" t="s">
+      <c r="D82" s="27"/>
+      <c r="E82" s="27"/>
+      <c r="F82" s="27"/>
+      <c r="G82" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="H82" s="26" t="s">
+      <c r="H82" s="27" t="s">
         <v>173</v>
       </c>
       <c r="I82" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="J82" s="26" t="s">
+      <c r="J82" s="27" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="83" spans="1:10">
-      <c r="A83" s="27"/>
-      <c r="B83" s="27"/>
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="27"/>
-      <c r="F83" s="27"/>
-      <c r="G83" s="27"/>
-      <c r="H83" s="27"/>
+      <c r="A83" s="28"/>
+      <c r="B83" s="28"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="28"/>
+      <c r="E83" s="28"/>
+      <c r="F83" s="28"/>
+      <c r="G83" s="28"/>
+      <c r="H83" s="28"/>
       <c r="I83" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="J83" s="27"/>
+      <c r="J83" s="28"/>
     </row>
     <row r="84" spans="1:10">
-      <c r="A84" s="27"/>
-      <c r="B84" s="27"/>
-      <c r="C84" s="27"/>
-      <c r="D84" s="27"/>
-      <c r="E84" s="27"/>
-      <c r="F84" s="27"/>
-      <c r="G84" s="27"/>
-      <c r="H84" s="27"/>
+      <c r="A84" s="28"/>
+      <c r="B84" s="28"/>
+      <c r="C84" s="28"/>
+      <c r="D84" s="28"/>
+      <c r="E84" s="28"/>
+      <c r="F84" s="28"/>
+      <c r="G84" s="28"/>
+      <c r="H84" s="28"/>
       <c r="I84" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="J84" s="27"/>
+      <c r="J84" s="28"/>
     </row>
     <row r="85" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A85" s="28"/>
-      <c r="B85" s="28"/>
-      <c r="C85" s="28"/>
-      <c r="D85" s="28"/>
-      <c r="E85" s="28"/>
-      <c r="F85" s="28"/>
-      <c r="G85" s="28"/>
-      <c r="H85" s="28"/>
+      <c r="A85" s="29"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="29"/>
+      <c r="E85" s="29"/>
+      <c r="F85" s="29"/>
+      <c r="G85" s="29"/>
+      <c r="H85" s="29"/>
       <c r="I85" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="J85" s="28"/>
+      <c r="J85" s="29"/>
     </row>
     <row r="86" spans="1:10" ht="15.75" thickBot="1">
       <c r="A86" s="13">
@@ -5612,262 +5687,262 @@
       </c>
     </row>
     <row r="87" spans="1:10">
-      <c r="A87" s="26">
+      <c r="A87" s="27">
         <v>47</v>
       </c>
-      <c r="B87" s="26" t="s">
+      <c r="B87" s="27" t="s">
         <v>257</v>
       </c>
-      <c r="C87" s="26" t="s">
+      <c r="C87" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="D87" s="26"/>
-      <c r="E87" s="26"/>
-      <c r="F87" s="26"/>
-      <c r="G87" s="26" t="s">
+      <c r="D87" s="27"/>
+      <c r="E87" s="27"/>
+      <c r="F87" s="27"/>
+      <c r="G87" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="H87" s="26" t="s">
+      <c r="H87" s="27" t="s">
         <v>173</v>
       </c>
       <c r="I87" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="J87" s="26" t="s">
+      <c r="J87" s="27" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="88" spans="1:10">
-      <c r="A88" s="27"/>
-      <c r="B88" s="27"/>
-      <c r="C88" s="27"/>
-      <c r="D88" s="27"/>
-      <c r="E88" s="27"/>
-      <c r="F88" s="27"/>
-      <c r="G88" s="27"/>
-      <c r="H88" s="27"/>
+      <c r="A88" s="28"/>
+      <c r="B88" s="28"/>
+      <c r="C88" s="28"/>
+      <c r="D88" s="28"/>
+      <c r="E88" s="28"/>
+      <c r="F88" s="28"/>
+      <c r="G88" s="28"/>
+      <c r="H88" s="28"/>
       <c r="I88" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="J88" s="27"/>
+      <c r="J88" s="28"/>
     </row>
     <row r="89" spans="1:10">
-      <c r="A89" s="27"/>
-      <c r="B89" s="27"/>
-      <c r="C89" s="27"/>
-      <c r="D89" s="27"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="27"/>
-      <c r="G89" s="27"/>
-      <c r="H89" s="27"/>
+      <c r="A89" s="28"/>
+      <c r="B89" s="28"/>
+      <c r="C89" s="28"/>
+      <c r="D89" s="28"/>
+      <c r="E89" s="28"/>
+      <c r="F89" s="28"/>
+      <c r="G89" s="28"/>
+      <c r="H89" s="28"/>
       <c r="I89" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="J89" s="27"/>
+      <c r="J89" s="28"/>
     </row>
     <row r="90" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A90" s="28"/>
-      <c r="B90" s="28"/>
-      <c r="C90" s="28"/>
-      <c r="D90" s="28"/>
-      <c r="E90" s="28"/>
-      <c r="F90" s="28"/>
-      <c r="G90" s="28"/>
-      <c r="H90" s="28"/>
+      <c r="A90" s="29"/>
+      <c r="B90" s="29"/>
+      <c r="C90" s="29"/>
+      <c r="D90" s="29"/>
+      <c r="E90" s="29"/>
+      <c r="F90" s="29"/>
+      <c r="G90" s="29"/>
+      <c r="H90" s="29"/>
       <c r="I90" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="J90" s="28"/>
+      <c r="J90" s="29"/>
     </row>
     <row r="91" spans="1:10">
-      <c r="A91" s="23">
+      <c r="A91" s="24">
         <v>48</v>
       </c>
-      <c r="B91" s="23" t="s">
+      <c r="B91" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="C91" s="23" t="s">
+      <c r="C91" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="D91" s="23"/>
-      <c r="E91" s="23"/>
-      <c r="F91" s="23"/>
-      <c r="G91" s="23" t="s">
+      <c r="D91" s="24"/>
+      <c r="E91" s="24"/>
+      <c r="F91" s="24"/>
+      <c r="G91" s="24" t="s">
         <v>180</v>
       </c>
-      <c r="H91" s="23" t="s">
+      <c r="H91" s="24" t="s">
         <v>173</v>
       </c>
       <c r="I91" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="J91" s="23" t="s">
+      <c r="J91" s="24" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="92" spans="1:10">
-      <c r="A92" s="24"/>
-      <c r="B92" s="24"/>
-      <c r="C92" s="24"/>
-      <c r="D92" s="24"/>
-      <c r="E92" s="24"/>
-      <c r="F92" s="24"/>
-      <c r="G92" s="24"/>
-      <c r="H92" s="24"/>
+      <c r="A92" s="25"/>
+      <c r="B92" s="25"/>
+      <c r="C92" s="25"/>
+      <c r="D92" s="25"/>
+      <c r="E92" s="25"/>
+      <c r="F92" s="25"/>
+      <c r="G92" s="25"/>
+      <c r="H92" s="25"/>
       <c r="I92" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="J92" s="24"/>
+      <c r="J92" s="25"/>
     </row>
     <row r="93" spans="1:10">
-      <c r="A93" s="24"/>
-      <c r="B93" s="24"/>
-      <c r="C93" s="24"/>
-      <c r="D93" s="24"/>
-      <c r="E93" s="24"/>
-      <c r="F93" s="24"/>
-      <c r="G93" s="24"/>
-      <c r="H93" s="24"/>
+      <c r="A93" s="25"/>
+      <c r="B93" s="25"/>
+      <c r="C93" s="25"/>
+      <c r="D93" s="25"/>
+      <c r="E93" s="25"/>
+      <c r="F93" s="25"/>
+      <c r="G93" s="25"/>
+      <c r="H93" s="25"/>
       <c r="I93" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="J93" s="24"/>
+      <c r="J93" s="25"/>
     </row>
     <row r="94" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A94" s="25"/>
-      <c r="B94" s="25"/>
-      <c r="C94" s="25"/>
-      <c r="D94" s="25"/>
-      <c r="E94" s="25"/>
-      <c r="F94" s="25"/>
-      <c r="G94" s="25"/>
-      <c r="H94" s="25"/>
+      <c r="A94" s="26"/>
+      <c r="B94" s="26"/>
+      <c r="C94" s="26"/>
+      <c r="D94" s="26"/>
+      <c r="E94" s="26"/>
+      <c r="F94" s="26"/>
+      <c r="G94" s="26"/>
+      <c r="H94" s="26"/>
       <c r="I94" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J94" s="25"/>
+      <c r="J94" s="26"/>
     </row>
     <row r="95" spans="1:10">
-      <c r="A95" s="26">
+      <c r="A95" s="27">
         <v>49</v>
       </c>
-      <c r="B95" s="26" t="s">
+      <c r="B95" s="27" t="s">
         <v>259</v>
       </c>
-      <c r="C95" s="26" t="s">
+      <c r="C95" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="D95" s="26"/>
-      <c r="E95" s="26"/>
-      <c r="F95" s="26"/>
-      <c r="G95" s="26" t="s">
+      <c r="D95" s="27"/>
+      <c r="E95" s="27"/>
+      <c r="F95" s="27"/>
+      <c r="G95" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="H95" s="26" t="s">
+      <c r="H95" s="27" t="s">
         <v>173</v>
       </c>
       <c r="I95" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="J95" s="26" t="s">
+      <c r="J95" s="27" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="96" spans="1:10">
-      <c r="A96" s="27"/>
-      <c r="B96" s="27"/>
-      <c r="C96" s="27"/>
-      <c r="D96" s="27"/>
-      <c r="E96" s="27"/>
-      <c r="F96" s="27"/>
-      <c r="G96" s="27"/>
-      <c r="H96" s="27"/>
+      <c r="A96" s="28"/>
+      <c r="B96" s="28"/>
+      <c r="C96" s="28"/>
+      <c r="D96" s="28"/>
+      <c r="E96" s="28"/>
+      <c r="F96" s="28"/>
+      <c r="G96" s="28"/>
+      <c r="H96" s="28"/>
       <c r="I96" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="J96" s="27"/>
+      <c r="J96" s="28"/>
     </row>
     <row r="97" spans="1:10">
-      <c r="A97" s="27"/>
-      <c r="B97" s="27"/>
-      <c r="C97" s="27"/>
-      <c r="D97" s="27"/>
-      <c r="E97" s="27"/>
-      <c r="F97" s="27"/>
-      <c r="G97" s="27"/>
-      <c r="H97" s="27"/>
+      <c r="A97" s="28"/>
+      <c r="B97" s="28"/>
+      <c r="C97" s="28"/>
+      <c r="D97" s="28"/>
+      <c r="E97" s="28"/>
+      <c r="F97" s="28"/>
+      <c r="G97" s="28"/>
+      <c r="H97" s="28"/>
       <c r="I97" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="J97" s="27"/>
+      <c r="J97" s="28"/>
     </row>
     <row r="98" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A98" s="28"/>
-      <c r="B98" s="28"/>
-      <c r="C98" s="28"/>
-      <c r="D98" s="28"/>
-      <c r="E98" s="28"/>
-      <c r="F98" s="28"/>
-      <c r="G98" s="28"/>
-      <c r="H98" s="28"/>
+      <c r="A98" s="29"/>
+      <c r="B98" s="29"/>
+      <c r="C98" s="29"/>
+      <c r="D98" s="29"/>
+      <c r="E98" s="29"/>
+      <c r="F98" s="29"/>
+      <c r="G98" s="29"/>
+      <c r="H98" s="29"/>
       <c r="I98" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="J98" s="28"/>
+      <c r="J98" s="29"/>
     </row>
     <row r="99" spans="1:10">
-      <c r="A99" s="23">
+      <c r="A99" s="24">
         <v>50</v>
       </c>
-      <c r="B99" s="23" t="s">
+      <c r="B99" s="24" t="s">
         <v>260</v>
       </c>
-      <c r="C99" s="23" t="s">
+      <c r="C99" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="D99" s="23"/>
-      <c r="E99" s="23"/>
-      <c r="F99" s="23"/>
-      <c r="G99" s="23" t="s">
+      <c r="D99" s="24"/>
+      <c r="E99" s="24"/>
+      <c r="F99" s="24"/>
+      <c r="G99" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="H99" s="23" t="s">
+      <c r="H99" s="24" t="s">
         <v>173</v>
       </c>
       <c r="I99" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="J99" s="23" t="s">
+      <c r="J99" s="24" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="100" spans="1:10">
-      <c r="A100" s="24"/>
-      <c r="B100" s="24"/>
-      <c r="C100" s="24"/>
-      <c r="D100" s="24"/>
-      <c r="E100" s="24"/>
-      <c r="F100" s="24"/>
-      <c r="G100" s="24"/>
-      <c r="H100" s="24"/>
+      <c r="A100" s="25"/>
+      <c r="B100" s="25"/>
+      <c r="C100" s="25"/>
+      <c r="D100" s="25"/>
+      <c r="E100" s="25"/>
+      <c r="F100" s="25"/>
+      <c r="G100" s="25"/>
+      <c r="H100" s="25"/>
       <c r="I100" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="J100" s="24"/>
+      <c r="J100" s="25"/>
     </row>
     <row r="101" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A101" s="25"/>
-      <c r="B101" s="25"/>
-      <c r="C101" s="25"/>
-      <c r="D101" s="25"/>
-      <c r="E101" s="25"/>
-      <c r="F101" s="25"/>
-      <c r="G101" s="25"/>
-      <c r="H101" s="25"/>
+      <c r="A101" s="26"/>
+      <c r="B101" s="26"/>
+      <c r="C101" s="26"/>
+      <c r="D101" s="26"/>
+      <c r="E101" s="26"/>
+      <c r="F101" s="26"/>
+      <c r="G101" s="26"/>
+      <c r="H101" s="26"/>
       <c r="I101" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="J101" s="25"/>
+      <c r="J101" s="26"/>
     </row>
     <row r="102" spans="1:10" ht="15.75" thickBot="1">
       <c r="A102" s="15">
@@ -5896,330 +5971,330 @@
       </c>
     </row>
     <row r="103" spans="1:10">
-      <c r="A103" s="23">
+      <c r="A103" s="24">
         <v>52</v>
       </c>
-      <c r="B103" s="23" t="s">
+      <c r="B103" s="24" t="s">
         <v>262</v>
       </c>
-      <c r="C103" s="23" t="s">
+      <c r="C103" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="D103" s="23"/>
-      <c r="E103" s="23"/>
-      <c r="F103" s="23"/>
-      <c r="G103" s="23" t="s">
+      <c r="D103" s="24"/>
+      <c r="E103" s="24"/>
+      <c r="F103" s="24"/>
+      <c r="G103" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="H103" s="23" t="s">
+      <c r="H103" s="24" t="s">
         <v>173</v>
       </c>
       <c r="I103" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="J103" s="23" t="s">
+      <c r="J103" s="24" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="104" spans="1:10">
-      <c r="A104" s="24"/>
-      <c r="B104" s="24"/>
-      <c r="C104" s="24"/>
-      <c r="D104" s="24"/>
-      <c r="E104" s="24"/>
-      <c r="F104" s="24"/>
-      <c r="G104" s="24"/>
-      <c r="H104" s="24"/>
+      <c r="A104" s="25"/>
+      <c r="B104" s="25"/>
+      <c r="C104" s="25"/>
+      <c r="D104" s="25"/>
+      <c r="E104" s="25"/>
+      <c r="F104" s="25"/>
+      <c r="G104" s="25"/>
+      <c r="H104" s="25"/>
       <c r="I104" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="J104" s="24"/>
+      <c r="J104" s="25"/>
     </row>
     <row r="105" spans="1:10">
-      <c r="A105" s="24"/>
-      <c r="B105" s="24"/>
-      <c r="C105" s="24"/>
-      <c r="D105" s="24"/>
-      <c r="E105" s="24"/>
-      <c r="F105" s="24"/>
-      <c r="G105" s="24"/>
-      <c r="H105" s="24"/>
+      <c r="A105" s="25"/>
+      <c r="B105" s="25"/>
+      <c r="C105" s="25"/>
+      <c r="D105" s="25"/>
+      <c r="E105" s="25"/>
+      <c r="F105" s="25"/>
+      <c r="G105" s="25"/>
+      <c r="H105" s="25"/>
       <c r="I105" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="J105" s="24"/>
+      <c r="J105" s="25"/>
     </row>
     <row r="106" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A106" s="25"/>
-      <c r="B106" s="25"/>
-      <c r="C106" s="25"/>
-      <c r="D106" s="25"/>
-      <c r="E106" s="25"/>
-      <c r="F106" s="25"/>
-      <c r="G106" s="25"/>
-      <c r="H106" s="25"/>
+      <c r="A106" s="26"/>
+      <c r="B106" s="26"/>
+      <c r="C106" s="26"/>
+      <c r="D106" s="26"/>
+      <c r="E106" s="26"/>
+      <c r="F106" s="26"/>
+      <c r="G106" s="26"/>
+      <c r="H106" s="26"/>
       <c r="I106" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J106" s="25"/>
+      <c r="J106" s="26"/>
     </row>
     <row r="107" spans="1:10">
-      <c r="A107" s="26">
+      <c r="A107" s="27">
         <v>53</v>
       </c>
-      <c r="B107" s="26" t="s">
+      <c r="B107" s="27" t="s">
         <v>263</v>
       </c>
-      <c r="C107" s="26" t="s">
+      <c r="C107" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="D107" s="26"/>
-      <c r="E107" s="26"/>
-      <c r="F107" s="26"/>
-      <c r="G107" s="26" t="s">
+      <c r="D107" s="27"/>
+      <c r="E107" s="27"/>
+      <c r="F107" s="27"/>
+      <c r="G107" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="H107" s="26" t="s">
+      <c r="H107" s="27" t="s">
         <v>173</v>
       </c>
       <c r="I107" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="J107" s="26" t="s">
+      <c r="J107" s="27" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="108" spans="1:10">
-      <c r="A108" s="27"/>
-      <c r="B108" s="27"/>
-      <c r="C108" s="27"/>
-      <c r="D108" s="27"/>
-      <c r="E108" s="27"/>
-      <c r="F108" s="27"/>
-      <c r="G108" s="27"/>
-      <c r="H108" s="27"/>
+      <c r="A108" s="28"/>
+      <c r="B108" s="28"/>
+      <c r="C108" s="28"/>
+      <c r="D108" s="28"/>
+      <c r="E108" s="28"/>
+      <c r="F108" s="28"/>
+      <c r="G108" s="28"/>
+      <c r="H108" s="28"/>
       <c r="I108" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="J108" s="27"/>
+      <c r="J108" s="28"/>
     </row>
     <row r="109" spans="1:10">
-      <c r="A109" s="27"/>
-      <c r="B109" s="27"/>
-      <c r="C109" s="27"/>
-      <c r="D109" s="27"/>
-      <c r="E109" s="27"/>
-      <c r="F109" s="27"/>
-      <c r="G109" s="27"/>
-      <c r="H109" s="27"/>
+      <c r="A109" s="28"/>
+      <c r="B109" s="28"/>
+      <c r="C109" s="28"/>
+      <c r="D109" s="28"/>
+      <c r="E109" s="28"/>
+      <c r="F109" s="28"/>
+      <c r="G109" s="28"/>
+      <c r="H109" s="28"/>
       <c r="I109" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="J109" s="27"/>
+      <c r="J109" s="28"/>
     </row>
     <row r="110" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A110" s="28"/>
-      <c r="B110" s="28"/>
-      <c r="C110" s="28"/>
-      <c r="D110" s="28"/>
-      <c r="E110" s="28"/>
-      <c r="F110" s="28"/>
-      <c r="G110" s="28"/>
-      <c r="H110" s="28"/>
-      <c r="I110" s="29" t="s">
+      <c r="A110" s="29"/>
+      <c r="B110" s="29"/>
+      <c r="C110" s="29"/>
+      <c r="D110" s="29"/>
+      <c r="E110" s="29"/>
+      <c r="F110" s="29"/>
+      <c r="G110" s="29"/>
+      <c r="H110" s="29"/>
+      <c r="I110" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="J110" s="28"/>
+      <c r="J110" s="29"/>
     </row>
     <row r="111" spans="1:10">
-      <c r="A111" s="23">
+      <c r="A111" s="24">
         <v>54</v>
       </c>
-      <c r="B111" s="23" t="s">
+      <c r="B111" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="C111" s="23" t="s">
+      <c r="C111" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="D111" s="23"/>
-      <c r="E111" s="23"/>
-      <c r="F111" s="23"/>
-      <c r="G111" s="23" t="s">
+      <c r="D111" s="24"/>
+      <c r="E111" s="24"/>
+      <c r="F111" s="24"/>
+      <c r="G111" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="H111" s="23" t="s">
+      <c r="H111" s="24" t="s">
         <v>173</v>
       </c>
       <c r="I111" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="J111" s="23" t="s">
+      <c r="J111" s="24" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="112" spans="1:10">
-      <c r="A112" s="24"/>
-      <c r="B112" s="24"/>
-      <c r="C112" s="24"/>
-      <c r="D112" s="24"/>
-      <c r="E112" s="24"/>
-      <c r="F112" s="24"/>
-      <c r="G112" s="24"/>
-      <c r="H112" s="24"/>
+      <c r="A112" s="25"/>
+      <c r="B112" s="25"/>
+      <c r="C112" s="25"/>
+      <c r="D112" s="25"/>
+      <c r="E112" s="25"/>
+      <c r="F112" s="25"/>
+      <c r="G112" s="25"/>
+      <c r="H112" s="25"/>
       <c r="I112" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="J112" s="24"/>
+      <c r="J112" s="25"/>
     </row>
     <row r="113" spans="1:10">
-      <c r="A113" s="24"/>
-      <c r="B113" s="24"/>
-      <c r="C113" s="24"/>
-      <c r="D113" s="24"/>
-      <c r="E113" s="24"/>
-      <c r="F113" s="24"/>
-      <c r="G113" s="24"/>
-      <c r="H113" s="24"/>
+      <c r="A113" s="25"/>
+      <c r="B113" s="25"/>
+      <c r="C113" s="25"/>
+      <c r="D113" s="25"/>
+      <c r="E113" s="25"/>
+      <c r="F113" s="25"/>
+      <c r="G113" s="25"/>
+      <c r="H113" s="25"/>
       <c r="I113" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="J113" s="24"/>
+      <c r="J113" s="25"/>
     </row>
     <row r="114" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A114" s="25"/>
-      <c r="B114" s="25"/>
-      <c r="C114" s="25"/>
-      <c r="D114" s="25"/>
-      <c r="E114" s="25"/>
-      <c r="F114" s="25"/>
-      <c r="G114" s="25"/>
-      <c r="H114" s="25"/>
+      <c r="A114" s="26"/>
+      <c r="B114" s="26"/>
+      <c r="C114" s="26"/>
+      <c r="D114" s="26"/>
+      <c r="E114" s="26"/>
+      <c r="F114" s="26"/>
+      <c r="G114" s="26"/>
+      <c r="H114" s="26"/>
       <c r="I114" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J114" s="25"/>
+      <c r="J114" s="26"/>
     </row>
     <row r="115" spans="1:10">
-      <c r="A115" s="26">
+      <c r="A115" s="27">
         <v>55</v>
       </c>
-      <c r="B115" s="26" t="s">
+      <c r="B115" s="27" t="s">
         <v>265</v>
       </c>
-      <c r="C115" s="26" t="s">
+      <c r="C115" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="D115" s="26"/>
-      <c r="E115" s="26"/>
-      <c r="F115" s="26"/>
-      <c r="G115" s="26" t="s">
+      <c r="D115" s="27"/>
+      <c r="E115" s="27"/>
+      <c r="F115" s="27"/>
+      <c r="G115" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="H115" s="26" t="s">
+      <c r="H115" s="27" t="s">
         <v>173</v>
       </c>
       <c r="I115" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="J115" s="26" t="s">
+      <c r="J115" s="27" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="116" spans="1:10">
-      <c r="A116" s="27"/>
-      <c r="B116" s="27"/>
-      <c r="C116" s="27"/>
-      <c r="D116" s="27"/>
-      <c r="E116" s="27"/>
-      <c r="F116" s="27"/>
-      <c r="G116" s="27"/>
-      <c r="H116" s="27"/>
+      <c r="A116" s="28"/>
+      <c r="B116" s="28"/>
+      <c r="C116" s="28"/>
+      <c r="D116" s="28"/>
+      <c r="E116" s="28"/>
+      <c r="F116" s="28"/>
+      <c r="G116" s="28"/>
+      <c r="H116" s="28"/>
       <c r="I116" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="J116" s="27"/>
+      <c r="J116" s="28"/>
     </row>
     <row r="117" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A117" s="28"/>
-      <c r="B117" s="28"/>
-      <c r="C117" s="28"/>
-      <c r="D117" s="28"/>
-      <c r="E117" s="28"/>
-      <c r="F117" s="28"/>
-      <c r="G117" s="28"/>
-      <c r="H117" s="28"/>
+      <c r="A117" s="29"/>
+      <c r="B117" s="29"/>
+      <c r="C117" s="29"/>
+      <c r="D117" s="29"/>
+      <c r="E117" s="29"/>
+      <c r="F117" s="29"/>
+      <c r="G117" s="29"/>
+      <c r="H117" s="29"/>
       <c r="I117" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="J117" s="28"/>
+      <c r="J117" s="29"/>
     </row>
     <row r="118" spans="1:10">
-      <c r="A118" s="23">
+      <c r="A118" s="24">
         <v>56</v>
       </c>
-      <c r="B118" s="23" t="s">
+      <c r="B118" s="24" t="s">
         <v>266</v>
       </c>
-      <c r="C118" s="23" t="s">
+      <c r="C118" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="D118" s="23"/>
-      <c r="E118" s="23"/>
-      <c r="F118" s="23"/>
-      <c r="G118" s="23" t="s">
+      <c r="D118" s="24"/>
+      <c r="E118" s="24"/>
+      <c r="F118" s="24"/>
+      <c r="G118" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="H118" s="23" t="s">
+      <c r="H118" s="24" t="s">
         <v>173</v>
       </c>
       <c r="I118" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="J118" s="23" t="s">
+      <c r="J118" s="24" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="119" spans="1:10">
-      <c r="A119" s="24"/>
-      <c r="B119" s="24"/>
-      <c r="C119" s="24"/>
-      <c r="D119" s="24"/>
-      <c r="E119" s="24"/>
-      <c r="F119" s="24"/>
-      <c r="G119" s="24"/>
-      <c r="H119" s="24"/>
+      <c r="A119" s="25"/>
+      <c r="B119" s="25"/>
+      <c r="C119" s="25"/>
+      <c r="D119" s="25"/>
+      <c r="E119" s="25"/>
+      <c r="F119" s="25"/>
+      <c r="G119" s="25"/>
+      <c r="H119" s="25"/>
       <c r="I119" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="J119" s="24"/>
+      <c r="J119" s="25"/>
     </row>
     <row r="120" spans="1:10">
-      <c r="A120" s="24"/>
-      <c r="B120" s="24"/>
-      <c r="C120" s="24"/>
-      <c r="D120" s="24"/>
-      <c r="E120" s="24"/>
-      <c r="F120" s="24"/>
-      <c r="G120" s="24"/>
-      <c r="H120" s="24"/>
+      <c r="A120" s="25"/>
+      <c r="B120" s="25"/>
+      <c r="C120" s="25"/>
+      <c r="D120" s="25"/>
+      <c r="E120" s="25"/>
+      <c r="F120" s="25"/>
+      <c r="G120" s="25"/>
+      <c r="H120" s="25"/>
       <c r="I120" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="J120" s="24"/>
+      <c r="J120" s="25"/>
     </row>
     <row r="121" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A121" s="25"/>
-      <c r="B121" s="25"/>
-      <c r="C121" s="25"/>
-      <c r="D121" s="25"/>
-      <c r="E121" s="25"/>
-      <c r="F121" s="25"/>
-      <c r="G121" s="25"/>
-      <c r="H121" s="25"/>
+      <c r="A121" s="26"/>
+      <c r="B121" s="26"/>
+      <c r="C121" s="26"/>
+      <c r="D121" s="26"/>
+      <c r="E121" s="26"/>
+      <c r="F121" s="26"/>
+      <c r="G121" s="26"/>
+      <c r="H121" s="26"/>
       <c r="I121" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J121" s="25"/>
+      <c r="J121" s="26"/>
     </row>
     <row r="122" spans="1:10" ht="15.75" thickBot="1">
       <c r="A122" s="15">
@@ -6247,7 +6322,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="29.25" thickBot="1">
+    <row r="123" spans="1:10" ht="15.75" thickBot="1">
       <c r="A123" s="13">
         <v>58</v>
       </c>
@@ -6274,284 +6349,59 @@
       </c>
     </row>
     <row r="124" spans="1:10">
-      <c r="A124" s="26">
+      <c r="A124" s="27">
         <v>59</v>
       </c>
-      <c r="B124" s="26" t="s">
+      <c r="B124" s="27" t="s">
         <v>269</v>
       </c>
-      <c r="C124" s="26" t="s">
+      <c r="C124" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="D124" s="26"/>
-      <c r="E124" s="26"/>
-      <c r="F124" s="26"/>
-      <c r="G124" s="26" t="s">
+      <c r="D124" s="27"/>
+      <c r="E124" s="27"/>
+      <c r="F124" s="27"/>
+      <c r="G124" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="H124" s="26"/>
+      <c r="H124" s="27"/>
       <c r="I124" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="J124" s="26" t="s">
+      <c r="J124" s="27" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="125" spans="1:10">
-      <c r="A125" s="27"/>
-      <c r="B125" s="27"/>
-      <c r="C125" s="27"/>
-      <c r="D125" s="27"/>
-      <c r="E125" s="27"/>
-      <c r="F125" s="27"/>
-      <c r="G125" s="27"/>
-      <c r="H125" s="27"/>
+      <c r="A125" s="28"/>
+      <c r="B125" s="28"/>
+      <c r="C125" s="28"/>
+      <c r="D125" s="28"/>
+      <c r="E125" s="28"/>
+      <c r="F125" s="28"/>
+      <c r="G125" s="28"/>
+      <c r="H125" s="28"/>
       <c r="I125" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="J125" s="27"/>
+      <c r="J125" s="28"/>
     </row>
     <row r="126" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A126" s="28"/>
-      <c r="B126" s="28"/>
-      <c r="C126" s="28"/>
-      <c r="D126" s="28"/>
-      <c r="E126" s="28"/>
-      <c r="F126" s="28"/>
-      <c r="G126" s="28"/>
-      <c r="H126" s="28"/>
-      <c r="I126" s="29" t="s">
+      <c r="A126" s="29"/>
+      <c r="B126" s="29"/>
+      <c r="C126" s="29"/>
+      <c r="D126" s="29"/>
+      <c r="E126" s="29"/>
+      <c r="F126" s="29"/>
+      <c r="G126" s="29"/>
+      <c r="H126" s="29"/>
+      <c r="I126" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="J126" s="28"/>
+      <c r="J126" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="243">
-    <mergeCell ref="J118:J121"/>
-    <mergeCell ref="A124:A126"/>
-    <mergeCell ref="B124:B126"/>
-    <mergeCell ref="C124:C126"/>
-    <mergeCell ref="D124:D126"/>
-    <mergeCell ref="E124:E126"/>
-    <mergeCell ref="F124:F126"/>
-    <mergeCell ref="G124:G126"/>
-    <mergeCell ref="H124:H126"/>
-    <mergeCell ref="J124:J126"/>
-    <mergeCell ref="H115:H117"/>
-    <mergeCell ref="J115:J117"/>
-    <mergeCell ref="A118:A121"/>
-    <mergeCell ref="B118:B121"/>
-    <mergeCell ref="C118:C121"/>
-    <mergeCell ref="D118:D121"/>
-    <mergeCell ref="E118:E121"/>
-    <mergeCell ref="F118:F121"/>
-    <mergeCell ref="G118:G121"/>
-    <mergeCell ref="H118:H121"/>
-    <mergeCell ref="G111:G114"/>
-    <mergeCell ref="H111:H114"/>
-    <mergeCell ref="J111:J114"/>
-    <mergeCell ref="A115:A117"/>
-    <mergeCell ref="B115:B117"/>
-    <mergeCell ref="C115:C117"/>
-    <mergeCell ref="D115:D117"/>
-    <mergeCell ref="E115:E117"/>
-    <mergeCell ref="F115:F117"/>
-    <mergeCell ref="G115:G117"/>
-    <mergeCell ref="A111:A114"/>
-    <mergeCell ref="B111:B114"/>
-    <mergeCell ref="C111:C114"/>
-    <mergeCell ref="D111:D114"/>
-    <mergeCell ref="E111:E114"/>
-    <mergeCell ref="F111:F114"/>
-    <mergeCell ref="J103:J106"/>
-    <mergeCell ref="A107:A110"/>
-    <mergeCell ref="B107:B110"/>
-    <mergeCell ref="C107:C110"/>
-    <mergeCell ref="D107:D110"/>
-    <mergeCell ref="E107:E110"/>
-    <mergeCell ref="F107:F110"/>
-    <mergeCell ref="G107:G110"/>
-    <mergeCell ref="H107:H110"/>
-    <mergeCell ref="J107:J110"/>
-    <mergeCell ref="H99:H101"/>
-    <mergeCell ref="J99:J101"/>
-    <mergeCell ref="A103:A106"/>
-    <mergeCell ref="B103:B106"/>
-    <mergeCell ref="C103:C106"/>
-    <mergeCell ref="D103:D106"/>
-    <mergeCell ref="E103:E106"/>
-    <mergeCell ref="F103:F106"/>
-    <mergeCell ref="G103:G106"/>
-    <mergeCell ref="H103:H106"/>
-    <mergeCell ref="G95:G98"/>
-    <mergeCell ref="H95:H98"/>
-    <mergeCell ref="J95:J98"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="C99:C101"/>
-    <mergeCell ref="D99:D101"/>
-    <mergeCell ref="E99:E101"/>
-    <mergeCell ref="F99:F101"/>
-    <mergeCell ref="G99:G101"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="B95:B98"/>
-    <mergeCell ref="C95:C98"/>
-    <mergeCell ref="D95:D98"/>
-    <mergeCell ref="E95:E98"/>
-    <mergeCell ref="F95:F98"/>
-    <mergeCell ref="J87:J90"/>
-    <mergeCell ref="A91:A94"/>
-    <mergeCell ref="B91:B94"/>
-    <mergeCell ref="C91:C94"/>
-    <mergeCell ref="D91:D94"/>
-    <mergeCell ref="E91:E94"/>
-    <mergeCell ref="F91:F94"/>
-    <mergeCell ref="G91:G94"/>
-    <mergeCell ref="H91:H94"/>
-    <mergeCell ref="J91:J94"/>
-    <mergeCell ref="H82:H85"/>
-    <mergeCell ref="J82:J85"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="B87:B90"/>
-    <mergeCell ref="C87:C90"/>
-    <mergeCell ref="D87:D90"/>
-    <mergeCell ref="E87:E90"/>
-    <mergeCell ref="F87:F90"/>
-    <mergeCell ref="G87:G90"/>
-    <mergeCell ref="H87:H90"/>
-    <mergeCell ref="G78:G81"/>
-    <mergeCell ref="H78:H81"/>
-    <mergeCell ref="J78:J81"/>
-    <mergeCell ref="A82:A85"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="C82:C85"/>
-    <mergeCell ref="D82:D85"/>
-    <mergeCell ref="E82:E85"/>
-    <mergeCell ref="F82:F85"/>
-    <mergeCell ref="G82:G85"/>
-    <mergeCell ref="A78:A81"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="C78:C81"/>
-    <mergeCell ref="D78:D81"/>
-    <mergeCell ref="E78:E81"/>
-    <mergeCell ref="F78:F81"/>
-    <mergeCell ref="J66:J69"/>
-    <mergeCell ref="A71:A75"/>
-    <mergeCell ref="B71:B75"/>
-    <mergeCell ref="C71:C75"/>
-    <mergeCell ref="D71:D75"/>
-    <mergeCell ref="E71:E75"/>
-    <mergeCell ref="F71:F75"/>
-    <mergeCell ref="G71:G75"/>
-    <mergeCell ref="H71:H75"/>
-    <mergeCell ref="J71:J75"/>
-    <mergeCell ref="H58:H61"/>
-    <mergeCell ref="J58:J61"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="D66:D69"/>
-    <mergeCell ref="E66:E69"/>
-    <mergeCell ref="F66:F69"/>
-    <mergeCell ref="G66:G69"/>
-    <mergeCell ref="H66:H69"/>
-    <mergeCell ref="G54:G57"/>
-    <mergeCell ref="H54:H57"/>
-    <mergeCell ref="J54:J57"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="D58:D61"/>
-    <mergeCell ref="E58:E61"/>
-    <mergeCell ref="F58:F61"/>
-    <mergeCell ref="G58:G61"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="D54:D57"/>
-    <mergeCell ref="E54:E57"/>
-    <mergeCell ref="F54:F57"/>
-    <mergeCell ref="J49:J50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="J51:J52"/>
-    <mergeCell ref="H46:H48"/>
-    <mergeCell ref="J46:J48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="G40:G43"/>
-    <mergeCell ref="H40:H43"/>
-    <mergeCell ref="J40:J43"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="D46:D48"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="G46:G48"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="F40:F43"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="J37:J38"/>
-    <mergeCell ref="H23:H26"/>
-    <mergeCell ref="J23:J26"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="J17:J21"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="D17:D21"/>
-    <mergeCell ref="E17:E21"/>
-    <mergeCell ref="F17:F21"/>
-    <mergeCell ref="G17:G21"/>
-    <mergeCell ref="H17:H21"/>
-    <mergeCell ref="G12:G16"/>
-    <mergeCell ref="H12:H16"/>
-    <mergeCell ref="J12:J16"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="D12:D16"/>
-    <mergeCell ref="E12:E16"/>
-    <mergeCell ref="F12:F16"/>
     <mergeCell ref="H7:H11"/>
     <mergeCell ref="J7:J11"/>
     <mergeCell ref="G2:G6"/>
@@ -6570,6 +6420,231 @@
     <mergeCell ref="D2:D6"/>
     <mergeCell ref="E2:E6"/>
     <mergeCell ref="F2:F6"/>
+    <mergeCell ref="G12:G16"/>
+    <mergeCell ref="H12:H16"/>
+    <mergeCell ref="J12:J16"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="E12:E16"/>
+    <mergeCell ref="F12:F16"/>
+    <mergeCell ref="J17:J21"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="D17:D21"/>
+    <mergeCell ref="E17:E21"/>
+    <mergeCell ref="F17:F21"/>
+    <mergeCell ref="G17:G21"/>
+    <mergeCell ref="H17:H21"/>
+    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="J23:J26"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="J37:J38"/>
+    <mergeCell ref="G40:G43"/>
+    <mergeCell ref="H40:H43"/>
+    <mergeCell ref="J40:J43"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="G46:G48"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="F40:F43"/>
+    <mergeCell ref="H46:H48"/>
+    <mergeCell ref="J46:J48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="J49:J50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="J51:J52"/>
+    <mergeCell ref="G54:G57"/>
+    <mergeCell ref="H54:H57"/>
+    <mergeCell ref="J54:J57"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="D58:D61"/>
+    <mergeCell ref="E58:E61"/>
+    <mergeCell ref="F58:F61"/>
+    <mergeCell ref="G58:G61"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="D54:D57"/>
+    <mergeCell ref="E54:E57"/>
+    <mergeCell ref="F54:F57"/>
+    <mergeCell ref="H58:H61"/>
+    <mergeCell ref="J58:J61"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="E66:E69"/>
+    <mergeCell ref="F66:F69"/>
+    <mergeCell ref="G66:G69"/>
+    <mergeCell ref="H66:H69"/>
+    <mergeCell ref="J66:J69"/>
+    <mergeCell ref="A71:A75"/>
+    <mergeCell ref="B71:B75"/>
+    <mergeCell ref="C71:C75"/>
+    <mergeCell ref="D71:D75"/>
+    <mergeCell ref="E71:E75"/>
+    <mergeCell ref="F71:F75"/>
+    <mergeCell ref="G71:G75"/>
+    <mergeCell ref="H71:H75"/>
+    <mergeCell ref="J71:J75"/>
+    <mergeCell ref="G78:G81"/>
+    <mergeCell ref="H78:H81"/>
+    <mergeCell ref="J78:J81"/>
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="C82:C85"/>
+    <mergeCell ref="D82:D85"/>
+    <mergeCell ref="E82:E85"/>
+    <mergeCell ref="F82:F85"/>
+    <mergeCell ref="G82:G85"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="C78:C81"/>
+    <mergeCell ref="D78:D81"/>
+    <mergeCell ref="E78:E81"/>
+    <mergeCell ref="F78:F81"/>
+    <mergeCell ref="H82:H85"/>
+    <mergeCell ref="J82:J85"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="B87:B90"/>
+    <mergeCell ref="C87:C90"/>
+    <mergeCell ref="D87:D90"/>
+    <mergeCell ref="E87:E90"/>
+    <mergeCell ref="F87:F90"/>
+    <mergeCell ref="G87:G90"/>
+    <mergeCell ref="H87:H90"/>
+    <mergeCell ref="J87:J90"/>
+    <mergeCell ref="A91:A94"/>
+    <mergeCell ref="B91:B94"/>
+    <mergeCell ref="C91:C94"/>
+    <mergeCell ref="D91:D94"/>
+    <mergeCell ref="E91:E94"/>
+    <mergeCell ref="F91:F94"/>
+    <mergeCell ref="G91:G94"/>
+    <mergeCell ref="H91:H94"/>
+    <mergeCell ref="J91:J94"/>
+    <mergeCell ref="G95:G98"/>
+    <mergeCell ref="H95:H98"/>
+    <mergeCell ref="J95:J98"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="C99:C101"/>
+    <mergeCell ref="D99:D101"/>
+    <mergeCell ref="E99:E101"/>
+    <mergeCell ref="F99:F101"/>
+    <mergeCell ref="G99:G101"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="B95:B98"/>
+    <mergeCell ref="C95:C98"/>
+    <mergeCell ref="D95:D98"/>
+    <mergeCell ref="E95:E98"/>
+    <mergeCell ref="F95:F98"/>
+    <mergeCell ref="H99:H101"/>
+    <mergeCell ref="J99:J101"/>
+    <mergeCell ref="A103:A106"/>
+    <mergeCell ref="B103:B106"/>
+    <mergeCell ref="C103:C106"/>
+    <mergeCell ref="D103:D106"/>
+    <mergeCell ref="E103:E106"/>
+    <mergeCell ref="F103:F106"/>
+    <mergeCell ref="G103:G106"/>
+    <mergeCell ref="H103:H106"/>
+    <mergeCell ref="J103:J106"/>
+    <mergeCell ref="A107:A110"/>
+    <mergeCell ref="B107:B110"/>
+    <mergeCell ref="C107:C110"/>
+    <mergeCell ref="D107:D110"/>
+    <mergeCell ref="E107:E110"/>
+    <mergeCell ref="F107:F110"/>
+    <mergeCell ref="G107:G110"/>
+    <mergeCell ref="H107:H110"/>
+    <mergeCell ref="J107:J110"/>
+    <mergeCell ref="G111:G114"/>
+    <mergeCell ref="H111:H114"/>
+    <mergeCell ref="J111:J114"/>
+    <mergeCell ref="A115:A117"/>
+    <mergeCell ref="B115:B117"/>
+    <mergeCell ref="C115:C117"/>
+    <mergeCell ref="D115:D117"/>
+    <mergeCell ref="E115:E117"/>
+    <mergeCell ref="F115:F117"/>
+    <mergeCell ref="G115:G117"/>
+    <mergeCell ref="A111:A114"/>
+    <mergeCell ref="B111:B114"/>
+    <mergeCell ref="C111:C114"/>
+    <mergeCell ref="D111:D114"/>
+    <mergeCell ref="E111:E114"/>
+    <mergeCell ref="F111:F114"/>
+    <mergeCell ref="H115:H117"/>
+    <mergeCell ref="J115:J117"/>
+    <mergeCell ref="A118:A121"/>
+    <mergeCell ref="B118:B121"/>
+    <mergeCell ref="C118:C121"/>
+    <mergeCell ref="D118:D121"/>
+    <mergeCell ref="E118:E121"/>
+    <mergeCell ref="F118:F121"/>
+    <mergeCell ref="G118:G121"/>
+    <mergeCell ref="H118:H121"/>
+    <mergeCell ref="J118:J121"/>
+    <mergeCell ref="A124:A126"/>
+    <mergeCell ref="B124:B126"/>
+    <mergeCell ref="C124:C126"/>
+    <mergeCell ref="D124:D126"/>
+    <mergeCell ref="E124:E126"/>
+    <mergeCell ref="F124:F126"/>
+    <mergeCell ref="G124:G126"/>
+    <mergeCell ref="H124:H126"/>
+    <mergeCell ref="J124:J126"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" display="http://timeslots.eu.nli.net/timeslots/users/?sort=id"/>
@@ -6590,14 +6665,187 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="33" customFormat="1" ht="33.75" customHeight="1">
+      <c r="B1" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>279</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>278</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="32"/>
+      <c r="B3" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="32"/>
+      <c r="B4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="42" customHeight="1">
+      <c r="A8" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A8:H8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>